<commit_message>
Added MATH 102 to data.xlsx
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F88EED-E80F-D74F-9B6D-E4270AAFB3CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A4D3E5-609F-FF4C-B5E0-1DECE86698AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="5" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="380" yWindow="860" windowWidth="28040" windowHeight="16940" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>number</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>course_x</t>
+  </si>
+  <si>
+    <t>Differential Calculus with Applications to Life Sciences</t>
+  </si>
+  <si>
+    <t>Functions, derivatives, optimization, growth and decay, discrete probability.</t>
   </si>
 </sst>
 </file>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA558D3A-1489-2E48-A14C-5F94B15C1134}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,6 +596,23 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1141,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D5E774-6755-684C-B2A6-0325506B6789}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add coordinates for MATH 263
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E49EE8-18EF-9641-9AAC-48E4AFB4D436}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0209283-89E5-674F-81CC-FCE560274223}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16440" activeTab="5" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -1449,9 +1449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA558D3A-1489-2E48-A14C-5F94B15C1134}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2948,7 +2946,7 @@
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4733,9 +4731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B521BB6-DE7E-F648-84B9-F67E5C6BF11B}">
   <dimension ref="A1:C334"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F333" sqref="F333"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8595,9 +8591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC045EC-A8A3-974C-9403-34BA5D62B768}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9037,8 +9031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D5E774-6755-684C-B2A6-0325506B6789}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10571,18 +10565,18 @@
         <v>263</v>
       </c>
       <c r="B81" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C81" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.6269501277589538</v>
       </c>
       <c r="E81" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.6541802475774405</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -10711,9 +10705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DE2127-F1A0-9D43-BB22-8321377E9C1D}">
   <dimension ref="A1:G334"/>
   <sheetViews>
-    <sheetView topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="E284" sqref="E284"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14280,11 +14272,11 @@
       </c>
       <c r="F119" s="1">
         <f>VLOOKUP(C119,LayoutCourses!A:E,4,0)</f>
-        <v>0</v>
+        <v>1.6269501277589538</v>
       </c>
       <c r="G119" s="1">
         <f>VLOOKUP(C119,LayoutCourses!A:E,5,0)</f>
-        <v>0</v>
+        <v>3.6541802475774405</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Tracks and CoursesTracks sheet to data spreadsheet.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F5DB4B-2890-844F-A4B4-0664B63036F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07303C6D-E359-D74F-969E-C193B5801151}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16440" activeTab="5" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16440" activeTab="8" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="LayoutCourses" sheetId="5" r:id="rId6"/>
     <sheet name="LayoutRequisites" sheetId="8" r:id="rId7"/>
     <sheet name="Tracks" sheetId="4" r:id="rId8"/>
+    <sheet name="CoursesTracks" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="LayoutRequisites" localSheetId="6">LayoutRequisites!$A$1:$G$190</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="315">
   <si>
     <t>number</t>
   </si>
@@ -159,9 +160,6 @@
   </si>
   <si>
     <t>MATH 404, 541</t>
-  </si>
-  <si>
-    <t>Mathematic of Information</t>
   </si>
   <si>
     <t>x</t>
@@ -1048,6 +1046,30 @@
   </si>
   <si>
     <t>One of MATH 361, MATH 345.</t>
+  </si>
+  <si>
+    <t>Mathematics of Information</t>
+  </si>
+  <si>
+    <t>Mathematics of Discrete Algorithms</t>
+  </si>
+  <si>
+    <t>Mathematical Biology</t>
+  </si>
+  <si>
+    <t>Applied Track for Graduate School</t>
+  </si>
+  <si>
+    <t>Mathematical Modelling and Copmutation</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Mathematical Optimization</t>
+  </si>
+  <si>
+    <t>track_id</t>
   </si>
 </sst>
 </file>
@@ -1122,58 +1144,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1556,10 +1527,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
         <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1573,10 +1544,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
         <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1590,10 +1561,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -1607,10 +1578,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
         <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>54</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -1624,13 +1595,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
         <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1641,13 +1612,13 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
         <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1658,13 +1629,13 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1675,13 +1646,13 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>62</v>
-      </c>
-      <c r="E11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1692,13 +1663,13 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
         <v>64</v>
       </c>
-      <c r="D12" t="s">
-        <v>65</v>
-      </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1709,13 +1680,13 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
         <v>66</v>
       </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1726,13 +1697,13 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>69</v>
-      </c>
-      <c r="E14" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1743,10 +1714,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
         <v>71</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -1760,13 +1731,13 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
         <v>73</v>
-      </c>
-      <c r="E16" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1777,10 +1748,10 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
         <v>75</v>
-      </c>
-      <c r="D17" t="s">
-        <v>76</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -1794,13 +1765,13 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
         <v>77</v>
       </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1811,10 +1782,10 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
         <v>79</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -1828,10 +1799,10 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
         <v>81</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
@@ -1845,10 +1816,10 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
@@ -1862,10 +1833,10 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
         <v>84</v>
-      </c>
-      <c r="D22" t="s">
-        <v>85</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -1879,10 +1850,10 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
         <v>86</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -1896,10 +1867,10 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" t="s">
         <v>88</v>
-      </c>
-      <c r="D24" t="s">
-        <v>89</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -1913,10 +1884,10 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" t="s">
         <v>90</v>
-      </c>
-      <c r="D25" t="s">
-        <v>91</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
@@ -1930,13 +1901,13 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
         <v>92</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>93</v>
-      </c>
-      <c r="E26" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1947,10 +1918,10 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
@@ -1964,10 +1935,10 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
         <v>96</v>
-      </c>
-      <c r="D28" t="s">
-        <v>97</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
@@ -1981,10 +1952,10 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
         <v>98</v>
-      </c>
-      <c r="D29" t="s">
-        <v>99</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -1998,13 +1969,13 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" t="s">
         <v>100</v>
       </c>
-      <c r="D30" t="s">
-        <v>101</v>
-      </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2015,13 +1986,13 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
         <v>102</v>
       </c>
-      <c r="D31" t="s">
-        <v>103</v>
-      </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2032,10 +2003,10 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
@@ -2049,10 +2020,10 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
         <v>106</v>
-      </c>
-      <c r="D33" t="s">
-        <v>107</v>
       </c>
       <c r="E33" t="s">
         <v>7</v>
@@ -2066,10 +2037,10 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" t="s">
         <v>108</v>
-      </c>
-      <c r="D34" t="s">
-        <v>109</v>
       </c>
       <c r="E34" t="s">
         <v>7</v>
@@ -2083,10 +2054,10 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" t="s">
         <v>110</v>
-      </c>
-      <c r="D35" t="s">
-        <v>111</v>
       </c>
       <c r="E35" t="s">
         <v>7</v>
@@ -2100,10 +2071,10 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" t="s">
         <v>112</v>
-      </c>
-      <c r="D36" t="s">
-        <v>113</v>
       </c>
       <c r="E36" t="s">
         <v>7</v>
@@ -2117,10 +2088,10 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
         <v>114</v>
-      </c>
-      <c r="D37" t="s">
-        <v>115</v>
       </c>
       <c r="E37" t="s">
         <v>7</v>
@@ -2134,10 +2105,10 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" t="s">
         <v>116</v>
-      </c>
-      <c r="D38" t="s">
-        <v>117</v>
       </c>
       <c r="E38" t="s">
         <v>7</v>
@@ -2151,10 +2122,10 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
         <v>118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
       </c>
       <c r="E39" t="s">
         <v>7</v>
@@ -2168,10 +2139,10 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
         <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>121</v>
       </c>
       <c r="E40" t="s">
         <v>7</v>
@@ -2185,13 +2156,13 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" t="s">
         <v>122</v>
       </c>
-      <c r="D41" t="s">
-        <v>123</v>
-      </c>
       <c r="E41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2202,10 +2173,10 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" t="s">
         <v>124</v>
-      </c>
-      <c r="D42" t="s">
-        <v>125</v>
       </c>
       <c r="E42" t="s">
         <v>7</v>
@@ -2219,10 +2190,10 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" t="s">
         <v>126</v>
-      </c>
-      <c r="D43" t="s">
-        <v>127</v>
       </c>
       <c r="E43" t="s">
         <v>7</v>
@@ -2236,10 +2207,10 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" t="s">
         <v>128</v>
-      </c>
-      <c r="D44" t="s">
-        <v>129</v>
       </c>
       <c r="E44" t="s">
         <v>7</v>
@@ -2253,10 +2224,10 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" t="s">
         <v>131</v>
-      </c>
-      <c r="D45" t="s">
-        <v>132</v>
       </c>
       <c r="E45" t="s">
         <v>7</v>
@@ -2270,10 +2241,10 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E46" t="s">
         <v>7</v>
@@ -2287,10 +2258,10 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" t="s">
         <v>134</v>
-      </c>
-      <c r="D47" t="s">
-        <v>135</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -2304,10 +2275,10 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" t="s">
         <v>136</v>
-      </c>
-      <c r="D48" t="s">
-        <v>137</v>
       </c>
       <c r="E48" t="s">
         <v>7</v>
@@ -2321,10 +2292,10 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" t="s">
         <v>138</v>
-      </c>
-      <c r="D49" t="s">
-        <v>139</v>
       </c>
       <c r="E49" t="s">
         <v>7</v>
@@ -2338,13 +2309,13 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" t="s">
         <v>140</v>
       </c>
-      <c r="D50" t="s">
-        <v>141</v>
-      </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2355,10 +2326,10 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" t="s">
         <v>142</v>
-      </c>
-      <c r="D51" t="s">
-        <v>143</v>
       </c>
       <c r="E51" t="s">
         <v>7</v>
@@ -2372,10 +2343,10 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" t="s">
         <v>144</v>
-      </c>
-      <c r="D52" t="s">
-        <v>145</v>
       </c>
       <c r="E52" t="s">
         <v>7</v>
@@ -2389,10 +2360,10 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" t="s">
         <v>146</v>
-      </c>
-      <c r="D53" t="s">
-        <v>147</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
@@ -2406,10 +2377,10 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" t="s">
         <v>148</v>
-      </c>
-      <c r="D54" t="s">
-        <v>149</v>
       </c>
       <c r="E54" t="s">
         <v>7</v>
@@ -2423,13 +2394,13 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" t="s">
         <v>150</v>
       </c>
-      <c r="D55" t="s">
-        <v>151</v>
-      </c>
       <c r="E55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2440,13 +2411,13 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" t="s">
+        <v>273</v>
+      </c>
+      <c r="E56" t="s">
         <v>152</v>
-      </c>
-      <c r="D56" t="s">
-        <v>274</v>
-      </c>
-      <c r="E56" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2457,10 +2428,10 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" t="s">
         <v>154</v>
-      </c>
-      <c r="D57" t="s">
-        <v>155</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
@@ -2474,10 +2445,10 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" t="s">
         <v>156</v>
-      </c>
-      <c r="D58" t="s">
-        <v>157</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
@@ -2491,10 +2462,10 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" t="s">
         <v>158</v>
-      </c>
-      <c r="D59" t="s">
-        <v>159</v>
       </c>
       <c r="E59" t="s">
         <v>7</v>
@@ -2508,10 +2479,10 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
+        <v>159</v>
+      </c>
+      <c r="D60" t="s">
         <v>160</v>
-      </c>
-      <c r="D60" t="s">
-        <v>161</v>
       </c>
       <c r="E60" t="s">
         <v>7</v>
@@ -2525,10 +2496,10 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D61" t="s">
         <v>162</v>
-      </c>
-      <c r="D61" t="s">
-        <v>163</v>
       </c>
       <c r="E61" t="s">
         <v>7</v>
@@ -2542,10 +2513,10 @@
         <v>3</v>
       </c>
       <c r="C62" t="s">
+        <v>163</v>
+      </c>
+      <c r="D62" t="s">
         <v>164</v>
-      </c>
-      <c r="D62" t="s">
-        <v>165</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2559,10 +2530,10 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D63" t="s">
         <v>166</v>
-      </c>
-      <c r="D63" t="s">
-        <v>167</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
@@ -2576,10 +2547,10 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
+        <v>167</v>
+      </c>
+      <c r="D64" t="s">
         <v>168</v>
-      </c>
-      <c r="D64" t="s">
-        <v>169</v>
       </c>
       <c r="E64" t="s">
         <v>7</v>
@@ -2593,10 +2564,10 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
+        <v>169</v>
+      </c>
+      <c r="D65" t="s">
         <v>170</v>
-      </c>
-      <c r="D65" t="s">
-        <v>171</v>
       </c>
       <c r="E65" t="s">
         <v>7</v>
@@ -2610,10 +2581,10 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
+        <v>171</v>
+      </c>
+      <c r="D66" t="s">
         <v>172</v>
-      </c>
-      <c r="D66" t="s">
-        <v>173</v>
       </c>
       <c r="E66" t="s">
         <v>7</v>
@@ -2627,13 +2598,13 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
+        <v>173</v>
+      </c>
+      <c r="D67" t="s">
         <v>174</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>175</v>
-      </c>
-      <c r="E67" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2644,10 +2615,10 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
+        <v>176</v>
+      </c>
+      <c r="D68" t="s">
         <v>177</v>
-      </c>
-      <c r="D68" t="s">
-        <v>178</v>
       </c>
       <c r="E68" t="s">
         <v>7</v>
@@ -2661,10 +2632,10 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
+        <v>178</v>
+      </c>
+      <c r="D69" t="s">
         <v>179</v>
-      </c>
-      <c r="D69" t="s">
-        <v>180</v>
       </c>
       <c r="E69" t="s">
         <v>7</v>
@@ -2678,10 +2649,10 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D70" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E70" t="s">
         <v>7</v>
@@ -2695,10 +2666,10 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E71" t="s">
         <v>7</v>
@@ -2712,10 +2683,10 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
+        <v>184</v>
+      </c>
+      <c r="D72" t="s">
         <v>185</v>
-      </c>
-      <c r="D72" t="s">
-        <v>186</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
@@ -2729,10 +2700,10 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" t="s">
         <v>187</v>
-      </c>
-      <c r="D73" t="s">
-        <v>188</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
@@ -2746,10 +2717,10 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
+        <v>188</v>
+      </c>
+      <c r="D74" t="s">
         <v>189</v>
-      </c>
-      <c r="D74" t="s">
-        <v>190</v>
       </c>
       <c r="E74" t="s">
         <v>7</v>
@@ -2763,10 +2734,10 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" t="s">
         <v>191</v>
-      </c>
-      <c r="D75" t="s">
-        <v>192</v>
       </c>
       <c r="E75" t="s">
         <v>7</v>
@@ -2780,10 +2751,10 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
+        <v>192</v>
+      </c>
+      <c r="D76" t="s">
         <v>193</v>
-      </c>
-      <c r="D76" t="s">
-        <v>194</v>
       </c>
       <c r="E76" t="s">
         <v>7</v>
@@ -2797,10 +2768,10 @@
         <v>3</v>
       </c>
       <c r="C77" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" t="s">
         <v>195</v>
-      </c>
-      <c r="D77" t="s">
-        <v>196</v>
       </c>
       <c r="E77" t="s">
         <v>7</v>
@@ -2814,10 +2785,10 @@
         <v>3</v>
       </c>
       <c r="C78" t="s">
+        <v>196</v>
+      </c>
+      <c r="D78" t="s">
         <v>197</v>
-      </c>
-      <c r="D78" t="s">
-        <v>198</v>
       </c>
       <c r="E78" t="s">
         <v>7</v>
@@ -2831,10 +2802,10 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
+        <v>199</v>
+      </c>
+      <c r="D79" t="s">
         <v>200</v>
-      </c>
-      <c r="D79" t="s">
-        <v>201</v>
       </c>
       <c r="E79" t="s">
         <v>7</v>
@@ -2848,10 +2819,10 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D80" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E80" t="s">
         <v>7</v>
@@ -2865,10 +2836,10 @@
         <v>3</v>
       </c>
       <c r="C81" t="s">
+        <v>202</v>
+      </c>
+      <c r="D81" t="s">
         <v>203</v>
-      </c>
-      <c r="D81" t="s">
-        <v>204</v>
       </c>
       <c r="E81" t="s">
         <v>7</v>
@@ -2882,10 +2853,10 @@
         <v>3</v>
       </c>
       <c r="C82" t="s">
+        <v>204</v>
+      </c>
+      <c r="D82" t="s">
         <v>205</v>
-      </c>
-      <c r="D82" t="s">
-        <v>206</v>
       </c>
       <c r="E82" t="s">
         <v>7</v>
@@ -2899,10 +2870,10 @@
         <v>3</v>
       </c>
       <c r="C83" t="s">
+        <v>206</v>
+      </c>
+      <c r="D83" t="s">
         <v>207</v>
-      </c>
-      <c r="D83" t="s">
-        <v>208</v>
       </c>
       <c r="E83" t="s">
         <v>7</v>
@@ -2916,10 +2887,10 @@
         <v>3</v>
       </c>
       <c r="C84" t="s">
+        <v>208</v>
+      </c>
+      <c r="D84" t="s">
         <v>209</v>
-      </c>
-      <c r="D84" t="s">
-        <v>210</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
@@ -2933,10 +2904,10 @@
         <v>3</v>
       </c>
       <c r="C85" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" t="s">
         <v>211</v>
-      </c>
-      <c r="D85" t="s">
-        <v>212</v>
       </c>
       <c r="E85" t="s">
         <v>7</v>
@@ -2950,10 +2921,10 @@
         <v>3</v>
       </c>
       <c r="C86" t="s">
+        <v>212</v>
+      </c>
+      <c r="D86" t="s">
         <v>213</v>
-      </c>
-      <c r="D86" t="s">
-        <v>214</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
@@ -2967,10 +2938,10 @@
         <v>3</v>
       </c>
       <c r="C87" t="s">
+        <v>214</v>
+      </c>
+      <c r="D87" t="s">
         <v>215</v>
-      </c>
-      <c r="D87" t="s">
-        <v>216</v>
       </c>
       <c r="E87" t="s">
         <v>7</v>
@@ -3065,7 +3036,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3076,10 +3047,10 @@
         <v>121</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3090,10 +3061,10 @@
         <v>121</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3107,7 +3078,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3121,7 +3092,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3135,7 +3106,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3149,7 +3120,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3163,7 +3134,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3177,7 +3148,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3191,7 +3162,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3202,10 +3173,10 @@
         <v>220</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3216,10 +3187,10 @@
         <v>220</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3230,10 +3201,10 @@
         <v>221</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3244,10 +3215,10 @@
         <v>221</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3258,10 +3229,10 @@
         <v>223</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3272,10 +3243,10 @@
         <v>223</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3286,10 +3257,10 @@
         <v>226</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3300,10 +3271,10 @@
         <v>226</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3317,7 +3288,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -3331,7 +3302,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3345,7 +3316,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3373,7 +3344,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3387,7 +3358,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -3401,7 +3372,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3415,7 +3386,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3429,7 +3400,7 @@
         <v>14</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3443,7 +3414,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3457,7 +3428,7 @@
         <v>13</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3471,7 +3442,7 @@
         <v>14</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3485,7 +3456,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3513,7 +3484,7 @@
         <v>13</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -3527,7 +3498,7 @@
         <v>14</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -3541,7 +3512,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -3555,7 +3526,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -3569,7 +3540,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -3583,7 +3554,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3597,7 +3568,7 @@
         <v>13</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -3611,7 +3582,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -3625,7 +3596,7 @@
         <v>14</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3639,7 +3610,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3650,10 +3621,10 @@
         <v>302</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3667,7 +3638,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -3681,7 +3652,7 @@
         <v>13</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -3695,7 +3666,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -3709,7 +3680,7 @@
         <v>14</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -3723,7 +3694,7 @@
         <v>13</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -3737,7 +3708,7 @@
         <v>13</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -3748,10 +3719,10 @@
         <v>308</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -3762,10 +3733,10 @@
         <v>308</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -3776,10 +3747,10 @@
         <v>309</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -3790,10 +3761,10 @@
         <v>309</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -3807,7 +3778,7 @@
         <v>13</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -3821,7 +3792,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -3835,7 +3806,7 @@
         <v>13</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -3849,7 +3820,7 @@
         <v>13</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -3863,7 +3834,7 @@
         <v>13</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -3877,7 +3848,7 @@
         <v>13</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -3888,10 +3859,10 @@
         <v>317</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -3905,7 +3876,7 @@
         <v>13</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -3919,7 +3890,7 @@
         <v>13</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -3933,7 +3904,7 @@
         <v>14</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -3944,10 +3915,10 @@
         <v>320</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -3958,10 +3929,10 @@
         <v>320</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -3975,7 +3946,7 @@
         <v>13</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -3986,10 +3957,10 @@
         <v>322</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -4000,10 +3971,10 @@
         <v>322</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -4017,7 +3988,7 @@
         <v>13</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -4031,7 +4002,7 @@
         <v>13</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -4045,7 +4016,7 @@
         <v>13</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -4056,10 +4027,10 @@
         <v>342</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -4070,10 +4041,10 @@
         <v>342</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -4084,10 +4055,10 @@
         <v>344</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -4098,10 +4069,10 @@
         <v>344</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -4115,7 +4086,7 @@
         <v>13</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -4129,7 +4100,7 @@
         <v>13</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -4143,7 +4114,7 @@
         <v>13</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -4157,7 +4128,7 @@
         <v>13</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -4171,7 +4142,7 @@
         <v>13</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -4182,10 +4153,10 @@
         <v>401</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -4196,10 +4167,10 @@
         <v>401</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -4213,7 +4184,7 @@
         <v>13</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -4227,7 +4198,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -4238,10 +4209,10 @@
         <v>403</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -4255,7 +4226,7 @@
         <v>13</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -4269,7 +4240,7 @@
         <v>14</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -4283,7 +4254,7 @@
         <v>13</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -4297,7 +4268,7 @@
         <v>13</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -4308,10 +4279,10 @@
         <v>406</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -4322,10 +4293,10 @@
         <v>406</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -4339,7 +4310,7 @@
         <v>13</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -4353,7 +4324,7 @@
         <v>13</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -4367,7 +4338,7 @@
         <v>13</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -4381,7 +4352,7 @@
         <v>13</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -4395,7 +4366,7 @@
         <v>13</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -4409,7 +4380,7 @@
         <v>13</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -4423,7 +4394,7 @@
         <v>13</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -4437,7 +4408,7 @@
         <v>13</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -4451,7 +4422,7 @@
         <v>13</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -4462,10 +4433,10 @@
         <v>424</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -4476,10 +4447,10 @@
         <v>424</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -4490,10 +4461,10 @@
         <v>424</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -4504,10 +4475,10 @@
         <v>424</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -4521,7 +4492,7 @@
         <v>13</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -4535,7 +4506,7 @@
         <v>13</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -4549,7 +4520,7 @@
         <v>13</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -4563,7 +4534,7 @@
         <v>13</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -4577,7 +4548,7 @@
         <v>13</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -4591,7 +4562,7 @@
         <v>14</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -4605,7 +4576,7 @@
         <v>14</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -4619,7 +4590,7 @@
         <v>13</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -4633,7 +4604,7 @@
         <v>13</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -4647,7 +4618,7 @@
         <v>13</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -4661,7 +4632,7 @@
         <v>13</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -4675,7 +4646,7 @@
         <v>13</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -4689,7 +4660,7 @@
         <v>13</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -4703,7 +4674,7 @@
         <v>13</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -4717,7 +4688,7 @@
         <v>13</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -4731,7 +4702,7 @@
         <v>13</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -4745,7 +4716,7 @@
         <v>13</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -4759,7 +4730,7 @@
         <v>13</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -4781,13 +4752,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -8640,7 +8611,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -9071,9 +9042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D5E774-6755-684C-B2A6-0325506B6789}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9087,16 +9056,16 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -10737,11 +10706,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E73">
     <sortCondition ref="A2:A73"/>
   </sortState>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10765,25 +10729,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -20783,9 +20747,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0A164B-708E-884A-B2CD-DB267B8D4A7F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20808,7 +20774,732 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5605FB08-D761-1B4B-8F7E-F0D219ED9D4B}">
+  <dimension ref="A1:B83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>6</v>
+      </c>
+      <c r="B59">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>6</v>
+      </c>
+      <c r="B60">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>6</v>
+      </c>
+      <c r="B66">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>6</v>
+      </c>
+      <c r="B68">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>6</v>
+      </c>
+      <c r="B69">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>7</v>
+      </c>
+      <c r="B71">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>7</v>
+      </c>
+      <c r="B72">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>7</v>
+      </c>
+      <c r="B73">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>7</v>
+      </c>
+      <c r="B74">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>7</v>
+      </c>
+      <c r="B75">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>7</v>
+      </c>
+      <c r="B76">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>7</v>
+      </c>
+      <c r="B77">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>7</v>
+      </c>
+      <c r="B78">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>7</v>
+      </c>
+      <c r="B79">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>7</v>
+      </c>
+      <c r="B80">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>7</v>
+      </c>
+      <c r="B81">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="B82">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>7</v>
+      </c>
+      <c r="B83">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create a dashboard layout and add requisite data to course info on hover
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8396A1F-A881-EB40-B8E4-93B002EFD8FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB658419-3EF8-164A-905E-50A25A80237B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="920" windowWidth="28040" windowHeight="16440" firstSheet="1" activeTab="10" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="440" yWindow="920" windowWidth="28040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="295">
   <si>
     <t>number</t>
   </si>
@@ -810,171 +810,36 @@
     <t>Honours Differential Calculus</t>
   </si>
   <si>
-    <t>One of MATH 100, MATH 102, MATH 104, MATH 110, MATH 120, MATH 180, MATH 184.</t>
-  </si>
-  <si>
-    <t>One of MATH 101, MATH 103, MATH 105, MATH 121, SCIE 001.</t>
-  </si>
-  <si>
     <t xml:space="preserve">One of MATH 215, MATH 255, MATH 256, MATH 258 </t>
   </si>
   <si>
-    <t>One of MATH 152, MATH 221, MATH 223.</t>
-  </si>
-  <si>
     <t>One of MATH 101, MATH 103, MATH 105, MATH 121, SCIE 001</t>
   </si>
   <si>
-    <t>One of MATH 200, MATH 217, MATH 226, MATH 253, MATH 254.</t>
-  </si>
-  <si>
     <t>One of MATH 152, MATH 221, MATH 223</t>
   </si>
   <si>
-    <t>A score of 68% or higher in MATH 226.</t>
-  </si>
-  <si>
-    <t>All of MECH 222, MECH 225.</t>
-  </si>
-  <si>
-    <t>One of MATH 101, MATH 103, MATH 105, MATH 121, SCIE 001 </t>
-  </si>
-  <si>
-    <t>One of MATH 215, MATH 255, MATH 256, MATH 258.</t>
-  </si>
-  <si>
-    <t>All of MECH 221, MECH 224.</t>
-  </si>
-  <si>
-    <t>One of BMEG 220, ELEC 211.</t>
-  </si>
-  <si>
-    <t>One of MATH 217, MATH 227, MATH 254, MATH 317.</t>
-  </si>
-  <si>
     <t>One of MATH 300, MATH 305</t>
   </si>
   <si>
-    <t>One of MATH 256, MATH 257, MATH 316, MATH 358, MECH 358, PHYS 312.</t>
-  </si>
-  <si>
-    <t>One of MATH 302, STAT 302.</t>
-  </si>
-  <si>
     <t>One of MATH 200, MATH 217, MATH 226, MATH 253, MATH 254</t>
   </si>
   <si>
-    <t>One of MATH 152, MATH 221, MATH 223 </t>
-  </si>
-  <si>
     <t>One of MATH 152, MATH 221</t>
   </si>
   <si>
-    <t>One of MATH 220, MATH 226, CPSC 121.</t>
-  </si>
-  <si>
-    <t>One of MATH 220, MATH 223, MATH 226, CPSC 121 and 9 additional credits of mathematics courses.</t>
-  </si>
-  <si>
-    <t>MATH 312.</t>
-  </si>
-  <si>
     <t>One of MATH 200, MATH 226, MATH 253</t>
   </si>
   <si>
-    <t>MATH 320.</t>
-  </si>
-  <si>
-    <t>MATH 322.</t>
-  </si>
-  <si>
-    <t>One of MATH 220, MATH 223, MATH 226, CPSC 121.</t>
-  </si>
-  <si>
-    <t>A score of 68% or higher in one of MATH 215, MATH 255, MATH 256, MATH 258.</t>
-  </si>
-  <si>
-    <t>One of BIOL 301, MATH 215, MATH 255, MATH 256, MATH 258.</t>
-  </si>
-  <si>
     <t>Fourier series; auto- and cross-correlation; power spectra; discrete Fourier transform; boundary-value problems; numerical methods; partial differential equations; heat, wave, Laplace, Poisson, and wave equations. Applications to mechanical engineering and practical computing applications emphasized. Credit will be granted for only one of MECH 358 or MATH 358. </t>
   </si>
   <si>
-    <t>A score of 68% or higher in one of MATH 301, MATH 320.</t>
-  </si>
-  <si>
-    <t>MATH 402 is recommended.</t>
-  </si>
-  <si>
-    <t>A score of 68% or higher in one of MATH 301, MATH 320. </t>
-  </si>
-  <si>
-    <t>MATH 420.</t>
-  </si>
-  <si>
     <t>One of MATH 307, CPSC 302</t>
   </si>
   <si>
-    <t>A score of 68% or higher in MATH 321.</t>
-  </si>
-  <si>
-    <t>MATH 418.</t>
-  </si>
-  <si>
-    <t>MATH 323.</t>
-  </si>
-  <si>
-    <t>A score of 68% or higher in one of MATH 412, MATH 422.</t>
-  </si>
-  <si>
-    <t>MATH 424.</t>
-  </si>
-  <si>
-    <t>A score of 68% or higher in all of MATH 321, MATH 322.</t>
-  </si>
-  <si>
-    <t>MATH 426.</t>
-  </si>
-  <si>
     <t>One of MATH 215, MATH 255, MATH 256, MATH 258</t>
   </si>
   <si>
-    <t>One of PHYS 216, PHYS 306, ENPH 270.</t>
-  </si>
-  <si>
-    <t>One of MATH 320, MATH 322.</t>
-  </si>
-  <si>
-    <t>MATH 300.</t>
-  </si>
-  <si>
-    <t>A score of 68% or higher in MATH 320.</t>
-  </si>
-  <si>
-    <t>MATH 340.</t>
-  </si>
-  <si>
-    <t>3rd year standing and one of MATH 220, MATH 223, MATH 226 or CPSC 221.</t>
-  </si>
-  <si>
-    <t>A score of 68% or higher in one of MATH 220, MATH 223, MATH 226, CPSC 121. And 6 credits of MATH numbered 300 or above.</t>
-  </si>
-  <si>
-    <t>One of MATH 220, MATH 226 and 6 credits of MATH courses numbered 300 or higher.</t>
-  </si>
-  <si>
-    <t>27 credits of MATH.</t>
-  </si>
-  <si>
-    <t>MATH 301.</t>
-  </si>
-  <si>
-    <t>MATH 400.</t>
-  </si>
-  <si>
-    <t>One of MATH 361, MATH 345.</t>
-  </si>
-  <si>
     <t>Mathematics of Information</t>
   </si>
   <si>
@@ -999,42 +864,9 @@
     <t>track_id</t>
   </si>
   <si>
-    <t>One of MATH 200, MATH 217, MATH 226, MATH 253.</t>
-  </si>
-  <si>
     <t>is_primary</t>
   </si>
   <si>
-    <t>Either (a) a score of 68% or higher in MATH 120 or (b) a score of 80% or higher in one of MATH 100, MATH 102, MATH 104, MATH 180, MATH 184 or (c) a score of 5 in AP Calculus AB.</t>
-  </si>
-  <si>
-    <t>A score of 68% or higher in MATH 322.</t>
-  </si>
-  <si>
-    <t>Either (a) a score of 64% or higher in one of MATH 101, MATH 103, MATH 105, SCIE 001 or (b) one of MATH 121, MATH 200, MATH 217, MATH 226, MATH 253, MATH 254.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Either (a) a score of 64% or higher in one of MATH 100, MATH 102, MATH 104, MATH 110, MATH 120, MATH 180, MATH 184 or (b) one of MATH 101, MATH 103, MATH 105, MATH 121, SCIE 001 </t>
-  </si>
-  <si>
-    <t>Either (a) MATH 121 or (b) a score of 68% or higher in one of MATH 101, MATH 103, MATH 105, SCIE 001.</t>
-  </si>
-  <si>
-    <t>Either (a) a score of 68% or higher in MATH 121 or (b) a score of 80% or higher in one of MATH 101, MATH 103, MATH 105, SCIE 001.</t>
-  </si>
-  <si>
-    <t>Either (a) one of MATH 152, MATH 221 and one of MATH 220, MATH 226, CPSC 121 or (b) MATH 223.</t>
-  </si>
-  <si>
-    <t>One of MATH 152, MATH 221, MATH 223 is recommended.</t>
-  </si>
-  <si>
-    <t>Either (a) a score of 68% or higher in MATH 226 or (b) one of MATH 200, MATH 217, MATH 226, MATH 253, MATH 254 and a score of 80% or higher in MATH 220.</t>
-  </si>
-  <si>
-    <t>Either (a) a score of 68% or higher in one of MATH 223, MATH 310 or (b) one of MATH 152, MATH 221, MATH 223 and a score of 80% or higher in MATH 220.</t>
-  </si>
-  <si>
     <t>Either (a) one of MATH 152, MATH 221 and one of MATH 220, MATH 226, CPSC 121 or (b) MATH 223</t>
   </si>
   <si>
@@ -1044,19 +876,157 @@
     <t>MATH 300 and a score of 68% or higher in MATH 321</t>
   </si>
   <si>
-    <t>Either (a) a score of 80% or higher in one of MATH 256, MATH 257, MATH 316, MATH 358, MECH 358, PHYS 312 or (b) MATH 400.</t>
-  </si>
-  <si>
     <t>Either (a) a score of 68% or higher in MATH 223 or (b) a score of 80% or higher in one of MATH 152, MATH 221</t>
   </si>
   <si>
-    <t>Either (a) a score of 68% or higher in MATH 227 or (b) a score of 80% or higher in one of MATH 217, MATH 254, MATH 264, MATH 317.</t>
-  </si>
-  <si>
     <t>requisite_is_primary</t>
   </si>
   <si>
-    <t>A score of 68% or higher in one of PHYS 102, PHYS 108, PHYS 118, PHYS 153, PHYS 158, SCIE 001 and a score of 68% or higher in one of MATH 101, MATH 103, MATH 105, MATH 121, SCIE 001.</t>
+    <t>Either (a) a score of 68% or higher in MATH 120 or (b) a score of 80% or higher in one of MATH 100, MATH 102, MATH 104, MATH 180, MATH 184 or (c) a score of 5 in AP Calculus AB</t>
+  </si>
+  <si>
+    <t>Either (a) a score of 64% or higher in one of MATH 101, MATH 103, MATH 105, SCIE 001 or (b) one of MATH 121, MATH 200, MATH 217, MATH 226, MATH 253, MATH 254</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in one of PHYS 102, PHYS 108, PHYS 118, PHYS 153, PHYS 158, SCIE 001 and a score of 68% or higher in one of MATH 101, MATH 103, MATH 105, MATH 121, SCIE 001</t>
+  </si>
+  <si>
+    <t>Either (a) a score of 64% or higher in one of MATH 100, MATH 102, MATH 104, MATH 110, MATH 120, MATH 180, MATH 184 or (b) one of MATH 101, MATH 103, MATH 105, MATH 121, SCIE 001</t>
+  </si>
+  <si>
+    <t>Either (a) MATH 121 or (b) a score of 68% or higher in one of MATH 101, MATH 103, MATH 105, SCIE 001</t>
+  </si>
+  <si>
+    <t>Either (a) a score of 68% or higher in MATH 121 or (b) a score of 80% or higher in one of MATH 101, MATH 103, MATH 105, SCIE 001</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in MATH 226</t>
+  </si>
+  <si>
+    <t>All of MECH 222, MECH 225</t>
+  </si>
+  <si>
+    <t>One of MATH 200, MATH 217, MATH 226, MATH 253</t>
+  </si>
+  <si>
+    <t>All of MECH 221, MECH 224</t>
+  </si>
+  <si>
+    <t>One of BMEG 220, ELEC 211</t>
+  </si>
+  <si>
+    <t>One of MATH 217, MATH 227, MATH 254, MATH 317</t>
+  </si>
+  <si>
+    <t>One of MATH 256, MATH 257, MATH 316, MATH 358, MECH 358, PHYS 312</t>
+  </si>
+  <si>
+    <t>One of MATH 302, STAT 302</t>
+  </si>
+  <si>
+    <t>One of MATH 220, MATH 226, CPSC 121</t>
+  </si>
+  <si>
+    <t>One of MATH 220, MATH 223, MATH 226, CPSC 121 and 9 additional credits of mathematics courses</t>
+  </si>
+  <si>
+    <t>MATH 312</t>
+  </si>
+  <si>
+    <t>One of MATH 152, MATH 221, MATH 223 is recommended</t>
+  </si>
+  <si>
+    <t>Either (a) a score of 68% or higher in MATH 226 or (b) one of MATH 200, MATH 217, MATH 226, MATH 253, MATH 254 and a score of 80% or higher in MATH 220</t>
+  </si>
+  <si>
+    <t>MATH 320</t>
+  </si>
+  <si>
+    <t>Either (a) a score of 68% or higher in one of MATH 223, MATH 310 or (b) one of MATH 152, MATH 221, MATH 223 and a score of 80% or higher in MATH 220</t>
+  </si>
+  <si>
+    <t>MATH 322</t>
+  </si>
+  <si>
+    <t>One of MATH 220, MATH 223, MATH 226, CPSC 121</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in one of MATH 215, MATH 255, MATH 256, MATH 258</t>
+  </si>
+  <si>
+    <t>One of BIOL 301, MATH 215, MATH 255, MATH 256, MATH 258</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in one of MATH 301, MATH 320</t>
+  </si>
+  <si>
+    <t>MATH 402 is recommended</t>
+  </si>
+  <si>
+    <t>MATH 420</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in MATH 320</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in MATH 322</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in MATH 321</t>
+  </si>
+  <si>
+    <t>MATH 418</t>
+  </si>
+  <si>
+    <t>MATH 323</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in one of MATH 412, MATH 422</t>
+  </si>
+  <si>
+    <t>Either (a) a score of 68% or higher in MATH 227 or (b) a score of 80% or higher in one of MATH 217, MATH 254, MATH 264, MATH 317</t>
+  </si>
+  <si>
+    <t>MATH 424</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in all of MATH 321, MATH 322</t>
+  </si>
+  <si>
+    <t>MATH 426</t>
+  </si>
+  <si>
+    <t>One of PHYS 216, PHYS 306, ENPH 270</t>
+  </si>
+  <si>
+    <t>One of MATH 320, MATH 322</t>
+  </si>
+  <si>
+    <t>MATH 300</t>
+  </si>
+  <si>
+    <t>MATH 340</t>
+  </si>
+  <si>
+    <t>3rd year standing and one of MATH 220, MATH 223, MATH 226 or CPSC 221</t>
+  </si>
+  <si>
+    <t>A score of 68% or higher in one of MATH 220, MATH 223, MATH 226, CPSC 121. And 6 credits of MATH numbered 300 or above</t>
+  </si>
+  <si>
+    <t>One of MATH 220, MATH 226 and 6 credits of MATH courses numbered 300 or higher</t>
+  </si>
+  <si>
+    <t>27 credits of MATH</t>
+  </si>
+  <si>
+    <t>MATH 301</t>
+  </si>
+  <si>
+    <t>MATH 400</t>
+  </si>
+  <si>
+    <t>One of MATH 361, MATH 345</t>
   </si>
 </sst>
 </file>
@@ -2407,7 +2377,7 @@
         <v>151</v>
       </c>
       <c r="D56" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="E56" t="s">
         <v>152</v>
@@ -4181,7 +4151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EEBBEA-02AB-3A44-9D7C-A60E65E1E2E4}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4212,7 +4182,7 @@
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>303</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -6804,8 +6774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC08885-D475-D740-B093-B1999F0EDA05}">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6884,7 +6854,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>222</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6898,7 +6868,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6940,7 +6910,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6954,7 +6924,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6968,7 +6938,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6982,7 +6952,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6996,7 +6966,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7010,7 +6980,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>289</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -7024,7 +6994,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>304</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7038,7 +7008,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -7052,7 +7022,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -7066,7 +7036,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -7080,7 +7050,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -7094,7 +7064,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -7108,7 +7078,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -7150,7 +7120,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -7164,7 +7134,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>230</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -7178,7 +7148,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -7192,7 +7162,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -7206,7 +7176,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -7220,7 +7190,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -7234,7 +7204,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -7248,7 +7218,7 @@
         <v>14</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -7262,7 +7232,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -7290,7 +7260,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -7304,7 +7274,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -7318,7 +7288,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -7332,7 +7302,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -7346,7 +7316,7 @@
         <v>13</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -7360,7 +7330,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -7374,7 +7344,7 @@
         <v>13</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -7388,7 +7358,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -7402,7 +7372,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -7416,7 +7386,7 @@
         <v>13</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -7430,7 +7400,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>238</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -7444,7 +7414,7 @@
         <v>13</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -7458,7 +7428,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -7472,7 +7442,7 @@
         <v>14</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -7486,7 +7456,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -7500,7 +7470,7 @@
         <v>13</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -7514,7 +7484,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>293</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -7528,7 +7498,7 @@
         <v>13</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>293</v>
+        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -7542,7 +7512,7 @@
         <v>13</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -7556,7 +7526,7 @@
         <v>13</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -7570,7 +7540,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -7584,7 +7554,7 @@
         <v>13</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -7598,7 +7568,7 @@
         <v>13</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -7612,7 +7582,7 @@
         <v>13</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -7626,7 +7596,7 @@
         <v>13</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -7640,7 +7610,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -7654,7 +7624,7 @@
         <v>13</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -7668,7 +7638,7 @@
         <v>14</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -7682,7 +7652,7 @@
         <v>13</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>295</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -7696,7 +7666,7 @@
         <v>13</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -7710,7 +7680,7 @@
         <v>13</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>296</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -7724,7 +7694,7 @@
         <v>13</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -7738,7 +7708,7 @@
         <v>13</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -7752,7 +7722,7 @@
         <v>13</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -7766,7 +7736,7 @@
         <v>13</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>297</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -7780,7 +7750,7 @@
         <v>13</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>297</v>
+        <v>241</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -7794,7 +7764,7 @@
         <v>13</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -7822,7 +7792,7 @@
         <v>13</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -7836,7 +7806,7 @@
         <v>13</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -7850,7 +7820,7 @@
         <v>13</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -7864,7 +7834,7 @@
         <v>13</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>298</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -7878,7 +7848,7 @@
         <v>13</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -7892,7 +7862,7 @@
         <v>13</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -7906,7 +7876,7 @@
         <v>13</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -7920,7 +7890,7 @@
         <v>13</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>299</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -7934,7 +7904,7 @@
         <v>14</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -7948,7 +7918,7 @@
         <v>13</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -7962,7 +7932,7 @@
         <v>13</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -7976,7 +7946,7 @@
         <v>13</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>300</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -7990,7 +7960,7 @@
         <v>13</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -8004,7 +7974,7 @@
         <v>13</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -8018,7 +7988,7 @@
         <v>13</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -8032,7 +8002,7 @@
         <v>13</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -8046,7 +8016,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -8060,7 +8030,7 @@
         <v>13</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -8074,7 +8044,7 @@
         <v>13</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -8088,7 +8058,7 @@
         <v>13</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -8102,7 +8072,7 @@
         <v>13</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -8116,7 +8086,7 @@
         <v>13</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>301</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -8130,7 +8100,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -8144,7 +8114,7 @@
         <v>13</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -8158,7 +8128,7 @@
         <v>13</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -8172,7 +8142,7 @@
         <v>13</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -8186,7 +8156,7 @@
         <v>13</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>264</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -8200,7 +8170,7 @@
         <v>13</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -8214,7 +8184,7 @@
         <v>14</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -8228,7 +8198,7 @@
         <v>14</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -8242,7 +8212,7 @@
         <v>13</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -8256,7 +8226,7 @@
         <v>13</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -8270,7 +8240,7 @@
         <v>13</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -8284,7 +8254,7 @@
         <v>13</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -8298,7 +8268,7 @@
         <v>13</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -8312,7 +8282,7 @@
         <v>13</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -8326,7 +8296,7 @@
         <v>13</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -8340,7 +8310,7 @@
         <v>13</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -8354,7 +8324,7 @@
         <v>13</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -8368,7 +8338,7 @@
         <v>13</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -8382,7 +8352,7 @@
         <v>13</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -8415,7 +8385,7 @@
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -13740,8 +13710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D5E774-6755-684C-B2A6-0325506B6789}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13779,11 +13749,11 @@
         <v>16</v>
       </c>
       <c r="D2" s="1">
-        <f>B2*COS(C2/32*3.14159)</f>
+        <f t="shared" ref="D2:D33" si="0">B2*COS(C2/32*3.14159)</f>
         <v>1.326794896677558E-6</v>
       </c>
       <c r="E2" s="1">
-        <f>B2*SIN(C2/32*3.14159)</f>
+        <f t="shared" ref="E2:E33" si="1">B2*SIN(C2/32*3.14159)</f>
         <v>0.99999999999911982</v>
       </c>
     </row>
@@ -13798,11 +13768,11 @@
         <v>16</v>
       </c>
       <c r="D3" s="1">
-        <f>B3*COS(C3/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>2.653589793355116E-6</v>
       </c>
       <c r="E3" s="1">
-        <f>B3*SIN(C3/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>1.9999999999982396</v>
       </c>
     </row>
@@ -13817,11 +13787,11 @@
         <v>28</v>
       </c>
       <c r="D4" s="1">
-        <f>B4*COS(C4/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-0.92387864395955233</v>
       </c>
       <c r="E4" s="1">
-        <f>B4*SIN(C4/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>0.38268557751169385</v>
       </c>
     </row>
@@ -13836,11 +13806,11 @@
         <v>28</v>
       </c>
       <c r="D5" s="1">
-        <f>B5*COS(C5/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-1.8477572879191047</v>
       </c>
       <c r="E5" s="1">
-        <f>B5*SIN(C5/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>0.76537115502338771</v>
       </c>
     </row>
@@ -13855,11 +13825,11 @@
         <v>34</v>
       </c>
       <c r="D6" s="1">
-        <f>B6*COS(C6/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-0.98078583044462497</v>
       </c>
       <c r="E6" s="1">
-        <f>B6*SIN(C6/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>-0.19508755675093026</v>
       </c>
     </row>
@@ -13874,11 +13844,11 @@
         <v>34</v>
       </c>
       <c r="D7" s="1">
-        <f>B7*COS(C7/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-1.9615716608892499</v>
       </c>
       <c r="E7" s="1">
-        <f>B7*SIN(C7/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>-0.39017511350186052</v>
       </c>
     </row>
@@ -13893,11 +13863,11 @@
         <v>46</v>
       </c>
       <c r="D8" s="1">
-        <f>B8*COS(C8/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-0.19509406325481018</v>
       </c>
       <c r="E8" s="1">
-        <f>B8*SIN(C8/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>-0.98078453621716943</v>
       </c>
     </row>
@@ -13912,11 +13882,11 @@
         <v>6</v>
       </c>
       <c r="D9" s="1">
-        <f>B9*COS(C9/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>0.83146988872534855</v>
       </c>
       <c r="E9" s="1">
-        <f>B9*SIN(C9/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>0.55556981932341898</v>
       </c>
     </row>
@@ -13931,11 +13901,11 @@
         <v>6</v>
       </c>
       <c r="D10" s="1">
-        <f>B10*COS(C10/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>1.6629397774506971</v>
       </c>
       <c r="E10" s="1">
-        <f>B10*SIN(C10/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>1.111139638646838</v>
       </c>
     </row>
@@ -13950,11 +13920,11 @@
         <v>10</v>
       </c>
       <c r="D11" s="1">
-        <f>B11*COS(C11/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>1.1111418450258703</v>
       </c>
       <c r="E11" s="1">
-        <f>B11*SIN(C11/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>1.6629383031948315</v>
       </c>
     </row>
@@ -13969,11 +13939,11 @@
         <v>22</v>
       </c>
       <c r="D12" s="1">
-        <f>B12*COS(C12/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-0.55556871613292513</v>
       </c>
       <c r="E12" s="1">
-        <f>B12*SIN(C12/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>0.83147062585181764</v>
       </c>
     </row>
@@ -13988,11 +13958,11 @@
         <v>40</v>
       </c>
       <c r="D13" s="1">
-        <f>B13*COS(C13/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-0.70710912664682912</v>
       </c>
       <c r="E13" s="1">
-        <f>B13*SIN(C13/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>-0.70710443571848602</v>
       </c>
     </row>
@@ -14007,11 +13977,11 @@
         <v>52</v>
       </c>
       <c r="D14" s="1">
-        <f>B14*COS(C14/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>0.38267944851592278</v>
       </c>
       <c r="E14" s="1">
-        <f>B14*SIN(C14/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>-0.92388118266557917</v>
       </c>
     </row>
@@ -14026,11 +13996,11 @@
         <v>16</v>
       </c>
       <c r="D15" s="1">
-        <f>B15*COS(C15/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>3.9803846900326745E-6</v>
       </c>
       <c r="E15" s="1">
-        <f>B15*SIN(C15/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>2.9999999999973594</v>
       </c>
     </row>
@@ -14045,11 +14015,11 @@
         <v>21</v>
       </c>
       <c r="D16" s="1">
-        <f>B16*COS(C16/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-1.8855808041258091</v>
       </c>
       <c r="E16" s="1">
-        <f>B16*SIN(C16/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>3.527688340983691</v>
       </c>
     </row>
@@ -14064,11 +14034,11 @@
         <v>14</v>
       </c>
       <c r="D17" s="1">
-        <f>B17*COS(C17/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>0.78036584261715414</v>
       </c>
       <c r="E17" s="1">
-        <f>B17*SIN(C17/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>3.923140215653325</v>
       </c>
     </row>
@@ -14083,11 +14053,11 @@
         <v>12</v>
       </c>
       <c r="D18" s="1">
-        <f>B18*COS(C18/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>1.3393952309986046</v>
       </c>
       <c r="E18" s="1">
-        <f>B18*SIN(C18/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>3.2335770309640366</v>
       </c>
     </row>
@@ -14096,18 +14066,18 @@
         <v>220</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1">
-        <f>B19*COS(C19/32*3.14159)</f>
-        <v>-2.8284214956265759</v>
+        <f t="shared" si="0"/>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E19" s="1">
-        <f>B19*SIN(C19/32*3.14159)</f>
-        <v>2.8284327538546012</v>
+        <f t="shared" si="1"/>
+        <v>1.66671607710442</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -14118,15 +14088,15 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="1">
-        <f>B20*COS(C20/32*3.14159)</f>
-        <v>-1.6667061483987755</v>
+        <f t="shared" si="0"/>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E20" s="1">
-        <f>B20*SIN(C20/32*3.14159)</f>
-        <v>2.4944118775554527</v>
+        <f t="shared" si="1"/>
+        <v>2.3190349899573843</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -14140,11 +14110,11 @@
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <f>B21*COS(C21/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E21" s="1">
-        <f>B21*SIN(C21/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -14159,11 +14129,11 @@
         <v>6</v>
       </c>
       <c r="D22" s="1">
-        <f>B22*COS(C22/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>2.4944096661760455</v>
       </c>
       <c r="E22" s="1">
-        <f>B22*SIN(C22/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>1.6667094579702568</v>
       </c>
     </row>
@@ -14175,15 +14145,15 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1">
-        <f>B23*COS(C23/32*3.14159)</f>
-        <v>3.3258795549013942</v>
+        <f t="shared" si="0"/>
+        <v>3.695518637787369</v>
       </c>
       <c r="E23" s="1">
-        <f>B23*SIN(C23/32*3.14159)</f>
-        <v>2.2222792772936759</v>
+        <f t="shared" si="1"/>
+        <v>1.5307325036616259</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -14197,11 +14167,11 @@
         <v>12</v>
       </c>
       <c r="D24" s="1">
-        <f>B24*COS(C24/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>1.148053055141661</v>
       </c>
       <c r="E24" s="1">
-        <f>B24*SIN(C24/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>2.7716374551120313</v>
       </c>
     </row>
@@ -14216,11 +14186,11 @@
         <v>12</v>
       </c>
       <c r="D25" s="1">
-        <f>B25*COS(C25/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>0.95671087928471765</v>
       </c>
       <c r="E25" s="1">
-        <f>B25*SIN(C25/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>2.309697879260026</v>
       </c>
     </row>
@@ -14235,11 +14205,11 @@
         <v>8</v>
       </c>
       <c r="D26" s="1">
-        <f>B26*COS(C26/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>2.1213217508376787</v>
       </c>
       <c r="E26" s="1">
-        <f>B26*SIN(C26/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>2.1213189362806726</v>
       </c>
     </row>
@@ -14254,11 +14224,11 @@
         <v>8</v>
       </c>
       <c r="D27" s="1">
-        <f>B27*COS(C27/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>2.4748753759772919</v>
       </c>
       <c r="E27" s="1">
-        <f>B27*SIN(C27/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>2.4748720923274514</v>
       </c>
     </row>
@@ -14273,11 +14243,11 @@
         <v>9</v>
       </c>
       <c r="D28" s="1">
-        <f>B28*COS(C28/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>2.5375754443131053</v>
       </c>
       <c r="E28" s="1">
-        <f>B28*SIN(C28/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>3.0920399196031001</v>
       </c>
     </row>
@@ -14292,11 +14262,11 @@
         <v>8</v>
       </c>
       <c r="D29" s="1">
-        <f>B29*COS(C29/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>1.7677681256980657</v>
       </c>
       <c r="E29" s="1">
-        <f>B29*SIN(C29/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>1.767765780233894</v>
       </c>
     </row>
@@ -14311,11 +14281,11 @@
         <v>11</v>
       </c>
       <c r="D30" s="1">
-        <f>B30*COS(C30/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>1.885590165156946</v>
       </c>
       <c r="E30" s="1">
-        <f>B30*SIN(C30/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>3.5276833374132948</v>
       </c>
     </row>
@@ -14330,11 +14300,11 @@
         <v>10</v>
       </c>
       <c r="D31" s="1">
-        <f>B31*COS(C31/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>2.7778546125646759</v>
       </c>
       <c r="E31" s="1">
-        <f>B31*SIN(C31/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>4.1573457579870787</v>
       </c>
     </row>
@@ -14349,11 +14319,11 @@
         <v>12</v>
       </c>
       <c r="D32" s="1">
-        <f>B32*COS(C32/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>2.296106110283322</v>
       </c>
       <c r="E32" s="1">
-        <f>B32*SIN(C32/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>5.5432749102240626</v>
       </c>
     </row>
@@ -14368,11 +14338,11 @@
         <v>17</v>
       </c>
       <c r="D33" s="1">
-        <f>B33*COS(C33/32*3.14159)</f>
+        <f t="shared" si="0"/>
         <v>-0.49007868699035295</v>
       </c>
       <c r="E33" s="1">
-        <f>B33*SIN(C33/32*3.14159)</f>
+        <f t="shared" si="1"/>
         <v>4.9759243242394486</v>
       </c>
     </row>
@@ -14387,11 +14357,11 @@
         <v>17</v>
       </c>
       <c r="D34" s="1">
-        <f>B34*COS(C34/32*3.14159)</f>
+        <f t="shared" ref="D34:D65" si="2">B34*COS(C34/32*3.14159)</f>
         <v>-0.58809442438842363</v>
       </c>
       <c r="E34" s="1">
-        <f>B34*SIN(C34/32*3.14159)</f>
+        <f t="shared" ref="E34:E65" si="3">B34*SIN(C34/32*3.14159)</f>
         <v>5.971109189087338</v>
       </c>
     </row>
@@ -14406,11 +14376,11 @@
         <v>10</v>
       </c>
       <c r="D35" s="1">
-        <f>B35*COS(C35/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>3.3334255350776107</v>
       </c>
       <c r="E35" s="1">
-        <f>B35*SIN(C35/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.9888149095844945</v>
       </c>
     </row>
@@ -14425,11 +14395,11 @@
         <v>18</v>
       </c>
       <c r="D36" s="1">
-        <f>B36*COS(C36/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-0.97544429026196555</v>
       </c>
       <c r="E36" s="1">
-        <f>B36*SIN(C36/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.9039278580129348</v>
       </c>
     </row>
@@ -14444,11 +14414,11 @@
         <v>28</v>
       </c>
       <c r="D37" s="1">
-        <f>B37*COS(C37/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-4.6193932197977619</v>
       </c>
       <c r="E37" s="1">
-        <f>B37*SIN(C37/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>1.9134278875584694</v>
       </c>
     </row>
@@ -14463,11 +14433,11 @@
         <v>27</v>
       </c>
       <c r="D38" s="1">
-        <f>B38*COS(C38/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-4.4096010445234768</v>
       </c>
       <c r="E38" s="1">
-        <f>B38*SIN(C38/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>2.3569935570844196</v>
       </c>
     </row>
@@ -14482,11 +14452,11 @@
         <v>26</v>
       </c>
       <c r="D39" s="1">
-        <f>B39*COS(C39/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-4.1573420723400947</v>
       </c>
       <c r="E39" s="1">
-        <f>B39*SIN(C39/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>2.777860128507367</v>
       </c>
     </row>
@@ -14501,11 +14471,11 @@
         <v>24</v>
       </c>
       <c r="D40" s="1">
-        <f>B40*COS(C40/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-3.5355268695332196</v>
       </c>
       <c r="E40" s="1">
-        <f>B40*SIN(C40/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>3.5355409423182516</v>
       </c>
     </row>
@@ -14520,11 +14490,11 @@
         <v>24</v>
       </c>
       <c r="D41" s="1">
-        <f>B41*COS(C41/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-4.2426322434398642</v>
       </c>
       <c r="E41" s="1">
-        <f>B41*SIN(C41/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.2426491307819019</v>
       </c>
     </row>
@@ -14539,11 +14509,11 @@
         <v>13</v>
       </c>
       <c r="D42" s="1">
-        <f>B42*COS(C42/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>1.4514285442796564</v>
       </c>
       <c r="E42" s="1">
-        <f>B42*SIN(C42/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.7847001139935861</v>
       </c>
     </row>
@@ -14558,11 +14528,11 @@
         <v>16</v>
       </c>
       <c r="D43" s="1">
-        <f>B43*COS(C43/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>6.6339744833877897E-6</v>
       </c>
       <c r="E43" s="1">
-        <f>B43*SIN(C43/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.9999999999955991</v>
       </c>
     </row>
@@ -14577,11 +14547,11 @@
         <v>16</v>
       </c>
       <c r="D44" s="1">
-        <f>B44*COS(C44/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>7.960769380065349E-6</v>
       </c>
       <c r="E44" s="1">
-        <f>B44*SIN(C44/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>5.9999999999947189</v>
       </c>
     </row>
@@ -14596,11 +14566,11 @@
         <v>6</v>
       </c>
       <c r="D45" s="1">
-        <f>B45*COS(C45/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>4.1573494436267424</v>
       </c>
       <c r="E45" s="1">
-        <f>B45*SIN(C45/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>2.777849096617095</v>
       </c>
     </row>
@@ -14615,11 +14585,11 @@
         <v>6</v>
       </c>
       <c r="D46" s="1">
-        <f>B46*COS(C46/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>4.9888193323520911</v>
       </c>
       <c r="E46" s="1">
-        <f>B46*SIN(C46/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>3.3334189159405136</v>
       </c>
     </row>
@@ -14634,11 +14604,11 @@
         <v>0</v>
       </c>
       <c r="D47" s="1">
-        <f>B47*COS(C47/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E47" s="1">
-        <f>B47*SIN(C47/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -14653,11 +14623,11 @@
         <v>0</v>
       </c>
       <c r="D48" s="1">
-        <f>B48*COS(C48/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E48" s="1">
-        <f>B48*SIN(C48/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -14672,11 +14642,11 @@
         <v>32</v>
       </c>
       <c r="D49" s="1">
-        <f>B49*COS(C49/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-4.9999999999823963</v>
       </c>
       <c r="E49" s="1">
-        <f>B49*SIN(C49/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>1.3267948966763902E-5</v>
       </c>
     </row>
@@ -14691,11 +14661,11 @@
         <v>19</v>
       </c>
       <c r="D50" s="1">
-        <f>B50*COS(C50/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-1.4514158476431596</v>
       </c>
       <c r="E50" s="1">
-        <f>B50*SIN(C50/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.784703965472711</v>
       </c>
     </row>
@@ -14710,11 +14680,11 @@
         <v>25</v>
       </c>
       <c r="D51" s="1">
-        <f>B51*COS(C51/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-3.8650456909477859</v>
       </c>
       <c r="E51" s="1">
-        <f>B51*SIN(C51/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>3.1719744335170716</v>
       </c>
     </row>
@@ -14729,11 +14699,11 @@
         <v>23</v>
       </c>
       <c r="D52" s="1">
-        <f>B52*COS(C52/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-3.1719590491232501</v>
       </c>
       <c r="E52" s="1">
-        <f>B52*SIN(C52/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>3.8650583165956403</v>
       </c>
     </row>
@@ -14748,11 +14718,11 @@
         <v>22</v>
       </c>
       <c r="D53" s="1">
-        <f>B53*COS(C53/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-2.7778435806646256</v>
       </c>
       <c r="E53" s="1">
-        <f>B53*SIN(C53/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.1573531292590884</v>
       </c>
     </row>
@@ -14767,11 +14737,11 @@
         <v>14</v>
       </c>
       <c r="D54" s="1">
-        <f>B54*COS(C54/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>0.97545730327144264</v>
       </c>
       <c r="E54" s="1">
-        <f>B54*SIN(C54/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>4.9039252695666562</v>
       </c>
     </row>
@@ -14786,11 +14756,11 @@
         <v>10</v>
       </c>
       <c r="D55" s="1">
-        <f>B55*COS(C55/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>2.3611764206799744</v>
       </c>
       <c r="E55" s="1">
-        <f>B55*SIN(C55/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>3.5337438942890169</v>
       </c>
     </row>
@@ -14805,11 +14775,11 @@
         <v>30</v>
       </c>
       <c r="D56" s="1">
-        <f>B56*COS(C56/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>-4.9039239753305681</v>
       </c>
       <c r="E56" s="1">
-        <f>B56*SIN(C56/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>0.97546380977360547</v>
       </c>
     </row>
@@ -14824,11 +14794,11 @@
         <v>15</v>
       </c>
       <c r="D57" s="1">
-        <f>B57*COS(C57/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>0.58811026926075216</v>
       </c>
       <c r="E57" s="1">
-        <f>B57*SIN(C57/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>5.9711076285049529</v>
       </c>
     </row>
@@ -14843,11 +14813,11 @@
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <f>B58*COS(C58/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>2.6787904619972092</v>
       </c>
       <c r="E58" s="1">
-        <f>B58*SIN(C58/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>6.4671540619280732</v>
       </c>
     </row>
@@ -14862,11 +14832,11 @@
         <v>12</v>
       </c>
       <c r="D59" s="1">
-        <f>B59*COS(C59/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>3.0614748137110963</v>
       </c>
       <c r="E59" s="1">
-        <f>B59*SIN(C59/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>7.3910332136320838</v>
       </c>
     </row>
@@ -14881,11 +14851,11 @@
         <v>9</v>
       </c>
       <c r="D60" s="1">
-        <f>B60*COS(C60/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>4.4407570275479342</v>
       </c>
       <c r="E60" s="1">
-        <f>B60*SIN(C60/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>5.4110698593054254</v>
       </c>
     </row>
@@ -14900,11 +14870,11 @@
         <v>9</v>
       </c>
       <c r="D61" s="1">
-        <f>B61*COS(C61/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>5.0751508886262107</v>
       </c>
       <c r="E61" s="1">
-        <f>B61*SIN(C61/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>6.1840798392062002</v>
       </c>
     </row>
@@ -14919,11 +14889,11 @@
         <v>8</v>
       </c>
       <c r="D62" s="1">
-        <f>B62*COS(C62/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>5.6568580022338102</v>
       </c>
       <c r="E62" s="1">
-        <f>B62*SIN(C62/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>5.6568504967484605</v>
       </c>
     </row>
@@ -14938,11 +14908,11 @@
         <v>13</v>
       </c>
       <c r="D63" s="1">
-        <f>B63*COS(C63/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>2.0319999619915192</v>
       </c>
       <c r="E63" s="1">
-        <f>B63*SIN(C63/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>6.698580159591021</v>
       </c>
     </row>
@@ -14957,11 +14927,11 @@
         <v>13</v>
       </c>
       <c r="D64" s="1">
-        <f>B64*COS(C64/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>2.3222856708474504</v>
       </c>
       <c r="E64" s="1">
-        <f>B64*SIN(C64/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>7.6555201823897381</v>
       </c>
     </row>
@@ -14976,11 +14946,11 @@
         <v>3</v>
       </c>
       <c r="D65" s="1">
-        <f>B65*COS(C65/32*3.14159)</f>
+        <f t="shared" si="2"/>
         <v>6.6985828556323046</v>
       </c>
       <c r="E65" s="1">
-        <f>B65*SIN(C65/32*3.14159)</f>
+        <f t="shared" si="3"/>
         <v>2.0319910743477587</v>
       </c>
     </row>
@@ -14995,11 +14965,11 @@
         <v>32</v>
       </c>
       <c r="D66" s="1">
-        <f>B66*COS(C66/32*3.14159)</f>
+        <f t="shared" ref="D66:D97" si="4">B66*COS(C66/32*3.14159)</f>
         <v>-6.9999999999753548</v>
       </c>
       <c r="E66" s="1">
-        <f>B66*SIN(C66/32*3.14159)</f>
+        <f t="shared" ref="E66:E86" si="5">B66*SIN(C66/32*3.14159)</f>
         <v>1.8575128553469462E-5</v>
       </c>
     </row>
@@ -15014,11 +14984,11 @@
         <v>7</v>
       </c>
       <c r="D67" s="1">
-        <f>B67*COS(C67/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>5.4110757512744234</v>
       </c>
       <c r="E67" s="1">
-        <f>B67*SIN(C67/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>4.4407498481641516</v>
       </c>
     </row>
@@ -15033,11 +15003,11 @@
         <v>7</v>
       </c>
       <c r="D68" s="1">
-        <f>B68*COS(C68/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>6.1840865728850556</v>
       </c>
       <c r="E68" s="1">
-        <f>B68*SIN(C68/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>5.075142683616173</v>
       </c>
     </row>
@@ -15052,11 +15022,11 @@
         <v>6</v>
       </c>
       <c r="D69" s="1">
-        <f>B69*COS(C69/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>5.8202892210774397</v>
       </c>
       <c r="E69" s="1">
-        <f>B69*SIN(C69/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>3.8889887352639327</v>
       </c>
     </row>
@@ -15071,11 +15041,11 @@
         <v>6</v>
       </c>
       <c r="D70" s="1">
-        <f>B70*COS(C70/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>6.6517591098027884</v>
       </c>
       <c r="E70" s="1">
-        <f>B70*SIN(C70/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>4.4445585545873518</v>
       </c>
     </row>
@@ -15090,11 +15060,11 @@
         <v>0</v>
       </c>
       <c r="D71" s="1">
-        <f>B71*COS(C71/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E71" s="1">
-        <f>B71*SIN(C71/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -15109,11 +15079,11 @@
         <v>0</v>
       </c>
       <c r="D72" s="1">
-        <f>B72*COS(C72/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="E72" s="1">
-        <f>B72*SIN(C72/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -15128,11 +15098,11 @@
         <v>4</v>
       </c>
       <c r="D73" s="1">
-        <f>B73*COS(C73/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>6.4671576161278956</v>
       </c>
       <c r="E73" s="1">
-        <f>B73*SIN(C73/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>2.6787818814078452</v>
       </c>
     </row>
@@ -15147,11 +15117,11 @@
         <v>4</v>
       </c>
       <c r="D74" s="1">
-        <f>B74*COS(C74/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>7.391037275574738</v>
       </c>
       <c r="E74" s="1">
-        <f>B74*SIN(C74/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>3.0614650073232519</v>
       </c>
     </row>
@@ -15166,11 +15136,11 @@
         <v>5</v>
       </c>
       <c r="D75" s="1">
-        <f>B75*COS(C75/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>6.1734502186027962</v>
       </c>
       <c r="E75" s="1">
-        <f>B75*SIN(C75/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>3.2997745981253157</v>
       </c>
     </row>
@@ -15185,11 +15155,11 @@
         <v>5</v>
       </c>
       <c r="D76" s="1">
-        <f>B76*COS(C76/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>7.0553716784031959</v>
       </c>
       <c r="E76" s="1">
-        <f>B76*SIN(C76/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>3.7711709692860751</v>
       </c>
     </row>
@@ -15204,11 +15174,11 @@
         <v>10</v>
       </c>
       <c r="D77" s="1">
-        <f>B77*COS(C77/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>3.888996457590546</v>
       </c>
       <c r="E77" s="1">
-        <f>B77*SIN(C77/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>5.8202840611819102</v>
       </c>
     </row>
@@ -15223,11 +15193,11 @@
         <v>1</v>
       </c>
       <c r="D78" s="1">
-        <f>B78*COS(C78/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>6.9662931436016358</v>
       </c>
       <c r="E78" s="1">
-        <f>B78*SIN(C78/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>0.68611940462928955</v>
       </c>
     </row>
@@ -15242,11 +15212,11 @@
         <v>11</v>
       </c>
       <c r="D79" s="1">
-        <f>B79*COS(C79/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>3.2997827890246554</v>
       </c>
       <c r="E79" s="1">
-        <f>B79*SIN(C79/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>6.1734458404732662</v>
       </c>
     </row>
@@ -15261,11 +15231,11 @@
         <v>19</v>
       </c>
       <c r="D80" s="1">
-        <f>B80*COS(C80/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>-2.0319821867004233</v>
       </c>
       <c r="E80" s="1">
-        <f>B80*SIN(C80/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>6.6985855516617958</v>
       </c>
     </row>
@@ -15277,15 +15247,15 @@
         <v>7</v>
       </c>
       <c r="C81">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D81" s="1">
-        <f>B81*COS(C81/32*3.14159)</f>
-        <v>-3.299766407220166</v>
+        <f t="shared" si="4"/>
+        <v>-5.4110639673268999</v>
       </c>
       <c r="E81" s="1">
-        <f>B81*SIN(C81/32*3.14159)</f>
-        <v>6.1734545967214594</v>
+        <f t="shared" si="5"/>
+        <v>4.4407642069239008</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -15299,11 +15269,11 @@
         <v>2</v>
       </c>
       <c r="D82" s="1">
-        <f>B82*COS(C82/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>6.8654971893117569</v>
       </c>
       <c r="E82" s="1">
-        <f>B82*SIN(C82/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>1.3656311154745873</v>
       </c>
     </row>
@@ -15315,15 +15285,15 @@
         <v>7</v>
       </c>
       <c r="C83">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D83" s="1">
-        <f>B83*COS(C83/32*3.14159)</f>
-        <v>-4.4407426687725504</v>
+        <f t="shared" si="4"/>
+        <v>-6.8654935654627955</v>
       </c>
       <c r="E83" s="1">
-        <f>B83*SIN(C83/32*3.14159)</f>
-        <v>5.4110816432338966</v>
+        <f t="shared" si="5"/>
+        <v>1.3656493336830475</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -15334,15 +15304,15 @@
         <v>7</v>
       </c>
       <c r="C84">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D84" s="1">
-        <f>B84*COS(C84/32*3.14159)</f>
-        <v>-5.4110639673268999</v>
+        <f t="shared" si="4"/>
+        <v>-6.4671505077168661</v>
       </c>
       <c r="E84" s="1">
-        <f>B84*SIN(C84/32*3.14159)</f>
-        <v>4.4407642069239008</v>
+        <f t="shared" si="5"/>
+        <v>2.6787990425818569</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -15356,11 +15326,11 @@
         <v>11</v>
       </c>
       <c r="D85" s="1">
-        <f>B85*COS(C85/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>3.771180330313892</v>
       </c>
       <c r="E85" s="1">
-        <f>B85*SIN(C85/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>7.0553666748265895</v>
       </c>
     </row>
@@ -15375,11 +15345,11 @@
         <v>15</v>
       </c>
       <c r="D86" s="1">
-        <f>B86*COS(C86/32*3.14159)</f>
+        <f t="shared" si="4"/>
         <v>0.68612864747087754</v>
       </c>
       <c r="E86" s="1">
-        <f>B86*SIN(C86/32*3.14159)</f>
+        <f t="shared" si="5"/>
         <v>6.9662922332557784</v>
       </c>
     </row>
@@ -15431,7 +15401,7 @@
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>303</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -16851,11 +16821,11 @@
       </c>
       <c r="F43" s="1">
         <f>VLOOKUP(C43,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G43" s="1">
         <f>VLOOKUP(C43,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H43">
         <f>CoursesRequisites!D43</f>
@@ -17089,11 +17059,11 @@
       </c>
       <c r="F50" s="1">
         <f>VLOOKUP(C50,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G50" s="1">
         <f>VLOOKUP(C50,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H50">
         <f>CoursesRequisites!D50</f>
@@ -17319,11 +17289,11 @@
       </c>
       <c r="D57" s="1">
         <f>VLOOKUP(B57,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E57" s="1">
         <f>VLOOKUP(B57,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F57" s="1">
         <f>VLOOKUP(C57,LayoutCourses!A:E,4,0)</f>
@@ -17353,11 +17323,11 @@
       </c>
       <c r="D58" s="1">
         <f>VLOOKUP(B58,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E58" s="1">
         <f>VLOOKUP(B58,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F58" s="1">
         <f>VLOOKUP(C58,LayoutCourses!A:E,4,0)</f>
@@ -17387,11 +17357,11 @@
       </c>
       <c r="D59" s="1">
         <f>VLOOKUP(B59,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E59" s="1">
         <f>VLOOKUP(B59,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F59" s="1">
         <f>VLOOKUP(C59,LayoutCourses!A:E,4,0)</f>
@@ -17421,11 +17391,11 @@
       </c>
       <c r="D60" s="1">
         <f>VLOOKUP(B60,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E60" s="1">
         <f>VLOOKUP(B60,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F60" s="1">
         <f>VLOOKUP(C60,LayoutCourses!A:E,4,0)</f>
@@ -17455,11 +17425,11 @@
       </c>
       <c r="D61" s="1">
         <f>VLOOKUP(B61,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E61" s="1">
         <f>VLOOKUP(B61,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F61" s="1">
         <f>VLOOKUP(C61,LayoutCourses!A:E,4,0)</f>
@@ -17489,11 +17459,11 @@
       </c>
       <c r="D62" s="1">
         <f>VLOOKUP(B62,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E62" s="1">
         <f>VLOOKUP(B62,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F62" s="1">
         <f>VLOOKUP(C62,LayoutCourses!A:E,4,0)</f>
@@ -17523,11 +17493,11 @@
       </c>
       <c r="D63" s="1">
         <f>VLOOKUP(B63,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E63" s="1">
         <f>VLOOKUP(B63,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F63" s="1">
         <f>VLOOKUP(C63,LayoutCourses!A:E,4,0)</f>
@@ -17557,11 +17527,11 @@
       </c>
       <c r="D64" s="1">
         <f>VLOOKUP(B64,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E64" s="1">
         <f>VLOOKUP(B64,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F64" s="1">
         <f>VLOOKUP(C64,LayoutCourses!A:E,4,0)</f>
@@ -17591,11 +17561,11 @@
       </c>
       <c r="D65" s="1">
         <f>VLOOKUP(B65,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="E65" s="1">
         <f>VLOOKUP(B65,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="F65" s="1">
         <f>VLOOKUP(C65,LayoutCourses!A:E,4,0)</f>
@@ -17803,11 +17773,11 @@
       </c>
       <c r="F71" s="1">
         <f>VLOOKUP(C71,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G71" s="1">
         <f>VLOOKUP(C71,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H71">
         <f>CoursesRequisites!D71</f>
@@ -17863,11 +17833,11 @@
       </c>
       <c r="D73" s="1">
         <f>VLOOKUP(B73,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E73" s="1">
         <f>VLOOKUP(B73,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F73" s="1">
         <f>VLOOKUP(C73,LayoutCourses!A:E,4,0)</f>
@@ -17897,11 +17867,11 @@
       </c>
       <c r="D74" s="1">
         <f>VLOOKUP(B74,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E74" s="1">
         <f>VLOOKUP(B74,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F74" s="1">
         <f>VLOOKUP(C74,LayoutCourses!A:E,4,0)</f>
@@ -17931,11 +17901,11 @@
       </c>
       <c r="D75" s="1">
         <f>VLOOKUP(B75,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E75" s="1">
         <f>VLOOKUP(B75,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F75" s="1">
         <f>VLOOKUP(C75,LayoutCourses!A:E,4,0)</f>
@@ -17965,11 +17935,11 @@
       </c>
       <c r="D76" s="1">
         <f>VLOOKUP(B76,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E76" s="1">
         <f>VLOOKUP(B76,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F76" s="1">
         <f>VLOOKUP(C76,LayoutCourses!A:E,4,0)</f>
@@ -17999,11 +17969,11 @@
       </c>
       <c r="D77" s="1">
         <f>VLOOKUP(B77,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E77" s="1">
         <f>VLOOKUP(B77,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F77" s="1">
         <f>VLOOKUP(C77,LayoutCourses!A:E,4,0)</f>
@@ -18033,11 +18003,11 @@
       </c>
       <c r="D78" s="1">
         <f>VLOOKUP(B78,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E78" s="1">
         <f>VLOOKUP(B78,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F78" s="1">
         <f>VLOOKUP(C78,LayoutCourses!A:E,4,0)</f>
@@ -18067,11 +18037,11 @@
       </c>
       <c r="D79" s="1">
         <f>VLOOKUP(B79,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E79" s="1">
         <f>VLOOKUP(B79,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F79" s="1">
         <f>VLOOKUP(C79,LayoutCourses!A:E,4,0)</f>
@@ -18101,11 +18071,11 @@
       </c>
       <c r="D80" s="1">
         <f>VLOOKUP(B80,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E80" s="1">
         <f>VLOOKUP(B80,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F80" s="1">
         <f>VLOOKUP(C80,LayoutCourses!A:E,4,0)</f>
@@ -18135,11 +18105,11 @@
       </c>
       <c r="D81" s="1">
         <f>VLOOKUP(B81,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E81" s="1">
         <f>VLOOKUP(B81,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F81" s="1">
         <f>VLOOKUP(C81,LayoutCourses!A:E,4,0)</f>
@@ -18169,11 +18139,11 @@
       </c>
       <c r="D82" s="1">
         <f>VLOOKUP(B82,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E82" s="1">
         <f>VLOOKUP(B82,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F82" s="1">
         <f>VLOOKUP(C82,LayoutCourses!A:E,4,0)</f>
@@ -18203,11 +18173,11 @@
       </c>
       <c r="D83" s="1">
         <f>VLOOKUP(B83,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="E83" s="1">
         <f>VLOOKUP(B83,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="F83" s="1">
         <f>VLOOKUP(C83,LayoutCourses!A:E,4,0)</f>
@@ -18551,11 +18521,11 @@
       </c>
       <c r="F93" s="1">
         <f>VLOOKUP(C93,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G93" s="1">
         <f>VLOOKUP(C93,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H93">
         <f>CoursesRequisites!D93</f>
@@ -18611,11 +18581,11 @@
       </c>
       <c r="D95" s="1">
         <f>VLOOKUP(B95,LayoutCourses!A:E,4,0)</f>
-        <v>3.3258795549013942</v>
+        <v>3.695518637787369</v>
       </c>
       <c r="E95" s="1">
         <f>VLOOKUP(B95,LayoutCourses!A:E,5,0)</f>
-        <v>2.2222792772936759</v>
+        <v>1.5307325036616259</v>
       </c>
       <c r="F95" s="1">
         <f>VLOOKUP(C95,LayoutCourses!A:E,4,0)</f>
@@ -18857,11 +18827,11 @@
       </c>
       <c r="F102" s="1">
         <f>VLOOKUP(C102,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G102" s="1">
         <f>VLOOKUP(C102,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H102">
         <f>CoursesRequisites!D102</f>
@@ -19095,11 +19065,11 @@
       </c>
       <c r="F109" s="1">
         <f>VLOOKUP(C109,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G109" s="1">
         <f>VLOOKUP(C109,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H109">
         <f>CoursesRequisites!D109</f>
@@ -19503,11 +19473,11 @@
       </c>
       <c r="F121" s="1">
         <f>VLOOKUP(C121,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G121" s="1">
         <f>VLOOKUP(C121,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H121">
         <f>CoursesRequisites!D121</f>
@@ -19911,11 +19881,11 @@
       </c>
       <c r="F133" s="1">
         <f>VLOOKUP(C133,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G133" s="1">
         <f>VLOOKUP(C133,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H133">
         <f>CoursesRequisites!D133</f>
@@ -20353,11 +20323,11 @@
       </c>
       <c r="F146" s="1">
         <f>VLOOKUP(C146,LayoutCourses!A:E,4,0)</f>
-        <v>3.3258795549013942</v>
+        <v>3.695518637787369</v>
       </c>
       <c r="G146" s="1">
         <f>VLOOKUP(C146,LayoutCourses!A:E,5,0)</f>
-        <v>2.2222792772936759</v>
+        <v>1.5307325036616259</v>
       </c>
       <c r="H146">
         <f>CoursesRequisites!D146</f>
@@ -21475,11 +21445,11 @@
       </c>
       <c r="F179" s="1">
         <f>VLOOKUP(C179,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G179" s="1">
         <f>VLOOKUP(C179,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H179">
         <f>CoursesRequisites!D179</f>
@@ -21747,11 +21717,11 @@
       </c>
       <c r="F187" s="1">
         <f>VLOOKUP(C187,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G187" s="1">
         <f>VLOOKUP(C187,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H187">
         <f>CoursesRequisites!D187</f>
@@ -21781,11 +21751,11 @@
       </c>
       <c r="F188" s="1">
         <f>VLOOKUP(C188,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G188" s="1">
         <f>VLOOKUP(C188,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H188">
         <f>CoursesRequisites!D188</f>
@@ -21917,11 +21887,11 @@
       </c>
       <c r="F192" s="1">
         <f>VLOOKUP(C192,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G192" s="1">
         <f>VLOOKUP(C192,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H192">
         <f>CoursesRequisites!D192</f>
@@ -21951,11 +21921,11 @@
       </c>
       <c r="F193" s="1">
         <f>VLOOKUP(C193,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G193" s="1">
         <f>VLOOKUP(C193,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H193">
         <f>CoursesRequisites!D193</f>
@@ -22087,11 +22057,11 @@
       </c>
       <c r="F197" s="1">
         <f>VLOOKUP(C197,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G197" s="1">
         <f>VLOOKUP(C197,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H197">
         <f>CoursesRequisites!D197</f>
@@ -22121,11 +22091,11 @@
       </c>
       <c r="F198" s="1">
         <f>VLOOKUP(C198,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G198" s="1">
         <f>VLOOKUP(C198,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H198">
         <f>CoursesRequisites!D198</f>
@@ -22189,11 +22159,11 @@
       </c>
       <c r="F200" s="1">
         <f>VLOOKUP(C200,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G200" s="1">
         <f>VLOOKUP(C200,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H200">
         <f>CoursesRequisites!D200</f>
@@ -22597,11 +22567,11 @@
       </c>
       <c r="F212" s="1">
         <f>VLOOKUP(C212,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G212" s="1">
         <f>VLOOKUP(C212,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H212">
         <f>CoursesRequisites!D212</f>
@@ -22699,11 +22669,11 @@
       </c>
       <c r="F215" s="1">
         <f>VLOOKUP(C215,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G215" s="1">
         <f>VLOOKUP(C215,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H215">
         <f>CoursesRequisites!D215</f>
@@ -23209,11 +23179,11 @@
       </c>
       <c r="F230" s="1">
         <f>VLOOKUP(C230,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G230" s="1">
         <f>VLOOKUP(C230,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H230">
         <f>CoursesRequisites!D230</f>
@@ -23379,11 +23349,11 @@
       </c>
       <c r="F235" s="1">
         <f>VLOOKUP(C235,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G235" s="1">
         <f>VLOOKUP(C235,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H235">
         <f>CoursesRequisites!D235</f>
@@ -23413,11 +23383,11 @@
       </c>
       <c r="F236" s="1">
         <f>VLOOKUP(C236,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G236" s="1">
         <f>VLOOKUP(C236,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H236">
         <f>CoursesRequisites!D236</f>
@@ -23515,11 +23485,11 @@
       </c>
       <c r="F239" s="1">
         <f>VLOOKUP(C239,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G239" s="1">
         <f>VLOOKUP(C239,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H239">
         <f>CoursesRequisites!D239</f>
@@ -23583,11 +23553,11 @@
       </c>
       <c r="F241" s="1">
         <f>VLOOKUP(C241,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G241" s="1">
         <f>VLOOKUP(C241,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H241">
         <f>CoursesRequisites!D241</f>
@@ -23719,11 +23689,11 @@
       </c>
       <c r="F245" s="1">
         <f>VLOOKUP(C245,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G245" s="1">
         <f>VLOOKUP(C245,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H245">
         <f>CoursesRequisites!D245</f>
@@ -23753,11 +23723,11 @@
       </c>
       <c r="F246" s="1">
         <f>VLOOKUP(C246,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G246" s="1">
         <f>VLOOKUP(C246,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H246">
         <f>CoursesRequisites!D246</f>
@@ -23889,11 +23859,11 @@
       </c>
       <c r="F250" s="1">
         <f>VLOOKUP(C250,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G250" s="1">
         <f>VLOOKUP(C250,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H250">
         <f>CoursesRequisites!D250</f>
@@ -23923,11 +23893,11 @@
       </c>
       <c r="F251" s="1">
         <f>VLOOKUP(C251,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G251" s="1">
         <f>VLOOKUP(C251,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H251">
         <f>CoursesRequisites!D251</f>
@@ -25827,11 +25797,11 @@
       </c>
       <c r="F307" s="1">
         <f>VLOOKUP(C307,LayoutCourses!A:E,4,0)</f>
-        <v>-1.6667061483987755</v>
+        <v>-1.9031754294739502</v>
       </c>
       <c r="G307" s="1">
         <f>VLOOKUP(C307,LayoutCourses!A:E,5,0)</f>
-        <v>2.4944118775554527</v>
+        <v>2.3190349899573843</v>
       </c>
       <c r="H307">
         <f>CoursesRequisites!D307</f>
@@ -25861,11 +25831,11 @@
       </c>
       <c r="F308" s="1">
         <f>VLOOKUP(C308,LayoutCourses!A:E,4,0)</f>
-        <v>3.3258795549013942</v>
+        <v>3.695518637787369</v>
       </c>
       <c r="G308" s="1">
         <f>VLOOKUP(C308,LayoutCourses!A:E,5,0)</f>
-        <v>2.2222792772936759</v>
+        <v>1.5307325036616259</v>
       </c>
       <c r="H308">
         <f>CoursesRequisites!D308</f>
@@ -26465,19 +26435,19 @@
       </c>
       <c r="D326" s="1">
         <f>VLOOKUP(B326,LayoutCourses!A:E,4,0)</f>
-        <v>-3.299766407220166</v>
+        <v>-5.4110639673268999</v>
       </c>
       <c r="E326" s="1">
         <f>VLOOKUP(B326,LayoutCourses!A:E,5,0)</f>
-        <v>6.1734545967214594</v>
+        <v>4.4407642069239008</v>
       </c>
       <c r="F326" s="1">
         <f>VLOOKUP(C326,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G326" s="1">
         <f>VLOOKUP(C326,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H326">
         <f>CoursesRequisites!D326</f>
@@ -26499,11 +26469,11 @@
       </c>
       <c r="D327" s="1">
         <f>VLOOKUP(B327,LayoutCourses!A:E,4,0)</f>
-        <v>-3.299766407220166</v>
+        <v>-5.4110639673268999</v>
       </c>
       <c r="E327" s="1">
         <f>VLOOKUP(B327,LayoutCourses!A:E,5,0)</f>
-        <v>6.1734545967214594</v>
+        <v>4.4407642069239008</v>
       </c>
       <c r="F327" s="1">
         <f>VLOOKUP(C327,LayoutCourses!A:E,4,0)</f>
@@ -26533,11 +26503,11 @@
       </c>
       <c r="D328" s="1">
         <f>VLOOKUP(B328,LayoutCourses!A:E,4,0)</f>
-        <v>-3.299766407220166</v>
+        <v>-5.4110639673268999</v>
       </c>
       <c r="E328" s="1">
         <f>VLOOKUP(B328,LayoutCourses!A:E,5,0)</f>
-        <v>6.1734545967214594</v>
+        <v>4.4407642069239008</v>
       </c>
       <c r="F328" s="1">
         <f>VLOOKUP(C328,LayoutCourses!A:E,4,0)</f>
@@ -26575,11 +26545,11 @@
       </c>
       <c r="F329" s="1">
         <f>VLOOKUP(C329,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G329" s="1">
         <f>VLOOKUP(C329,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H329">
         <f>CoursesRequisites!D329</f>
@@ -26669,19 +26639,19 @@
       </c>
       <c r="D332" s="1">
         <f>VLOOKUP(B332,LayoutCourses!A:E,4,0)</f>
-        <v>-4.4407426687725504</v>
+        <v>-6.8654935654627955</v>
       </c>
       <c r="E332" s="1">
         <f>VLOOKUP(B332,LayoutCourses!A:E,5,0)</f>
-        <v>5.4110816432338966</v>
+        <v>1.3656493336830475</v>
       </c>
       <c r="F332" s="1">
         <f>VLOOKUP(C332,LayoutCourses!A:E,4,0)</f>
-        <v>-2.8284214956265759</v>
+        <v>-2.4944052434040569</v>
       </c>
       <c r="G332" s="1">
         <f>VLOOKUP(C332,LayoutCourses!A:E,5,0)</f>
-        <v>2.8284327538546012</v>
+        <v>1.66671607710442</v>
       </c>
       <c r="H332">
         <f>CoursesRequisites!D332</f>
@@ -26703,11 +26673,11 @@
       </c>
       <c r="D333" s="1">
         <f>VLOOKUP(B333,LayoutCourses!A:E,4,0)</f>
-        <v>-4.4407426687725504</v>
+        <v>-6.8654935654627955</v>
       </c>
       <c r="E333" s="1">
         <f>VLOOKUP(B333,LayoutCourses!A:E,5,0)</f>
-        <v>5.4110816432338966</v>
+        <v>1.3656493336830475</v>
       </c>
       <c r="F333" s="1">
         <f>VLOOKUP(C333,LayoutCourses!A:E,4,0)</f>
@@ -26867,7 +26837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0A164B-708E-884A-B2CD-DB267B8D4A7F}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -26890,7 +26862,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -26898,7 +26870,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -26906,7 +26878,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -26914,7 +26886,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -26922,7 +26894,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -26930,7 +26902,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -26938,7 +26910,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -26950,13 +26922,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5605FB08-D761-1B4B-8F7E-F0D219ED9D4B}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:B46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Change dashboard layout with CSS grid
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A580822-93EF-A74E-8F13-2BC723372EAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ABA3C0-A4D5-DE4F-8589-0CE70CB77338}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="640" windowWidth="28040" windowHeight="16440" firstSheet="6" activeTab="14" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="400" yWindow="640" windowWidth="28040" windowHeight="16440" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="324">
   <si>
     <t>number</t>
   </si>
@@ -353,9 +353,6 @@
   </si>
   <si>
     <t>Multivariable and Vector Calculus</t>
-  </si>
-  <si>
-    <t>Partial differentiation, extreme values, multiple integration, vector fields, line and surface integrals, the divergence theorem, Green's and Stokes' theorems. Intended for students in Honours Physics and Engineering Physics. </t>
   </si>
   <si>
     <t>Mathematical Proof</t>
@@ -1096,6 +1093,78 @@
   <si>
     <t>BSc/BA Program</t>
   </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Intended for Honours students.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 550.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 508.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 527.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 525.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 502.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 501.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 537.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 510.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 507.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 545.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 544.</t>
+  </si>
+  <si>
+    <t>Intended for Honours students. Cross-listed with MATH 541.</t>
+  </si>
+  <si>
+    <t>Partial differentiation, extreme values, multiple integration, vector fields, line and surface integrals, the divergence theorem, Green's and Stokes' theorems.</t>
+  </si>
+  <si>
+    <t>Intended for students in Honours Physics and Engineering Physics.</t>
+  </si>
+  <si>
+    <t>Intended for non-math students. Math students are advised to take MATH 361 and 462.</t>
+  </si>
+  <si>
+    <t>Credit excluded with MATH 305.</t>
+  </si>
+  <si>
+    <t>Credited excluded with MATH 406.</t>
+  </si>
+  <si>
+    <t>Intended for Engineering Physics students. Credit excluded with both MATH 401 and MATH 405. Math students are advised to take MATH 401 and 405.</t>
+  </si>
+  <si>
+    <t>Intended for Engineering Physics students. Credit excluded with MATH 300. Math students are advised to take MATH 300.</t>
+  </si>
+  <si>
+    <t>Intended for Mechanical Engineering students.</t>
+  </si>
+  <si>
+    <t>For Mechanical Engineering students only.</t>
+  </si>
+  <si>
+    <t>Intended for students in Honours Physics and Engineering Physics.Credit excluded with MATH 227, 254, 264, and 317. Math students are advised to take MATH 317.</t>
+  </si>
 </sst>
 </file>
 
@@ -1499,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA558D3A-1489-2E48-A14C-5F94B15C1134}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,7 +1580,7 @@
     <col min="4" max="4" width="75.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1527,8 +1596,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -1545,7 +1617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>101</v>
       </c>
@@ -1562,7 +1634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>102</v>
       </c>
@@ -1579,7 +1651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>103</v>
       </c>
@@ -1596,7 +1668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>104</v>
       </c>
@@ -1613,7 +1685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>105</v>
       </c>
@@ -1630,7 +1702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>110</v>
       </c>
@@ -1638,7 +1710,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -1647,7 +1719,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>120</v>
       </c>
@@ -1655,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D9" t="s">
         <v>56</v>
@@ -1663,8 +1735,11 @@
       <c r="E9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>121</v>
       </c>
@@ -1680,8 +1755,11 @@
       <c r="E10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>152</v>
       </c>
@@ -1698,7 +1776,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>180</v>
       </c>
@@ -1715,7 +1793,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>184</v>
       </c>
@@ -1732,7 +1810,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>190</v>
       </c>
@@ -1749,7 +1827,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>200</v>
       </c>
@@ -1766,7 +1844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>210</v>
       </c>
@@ -1774,7 +1852,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D16" t="s">
         <v>72</v>
@@ -1783,7 +1861,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>215</v>
       </c>
@@ -1800,7 +1878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>217</v>
       </c>
@@ -1811,13 +1889,16 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>314</v>
       </c>
       <c r="E18" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>220</v>
       </c>
@@ -1825,16 +1906,16 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
         <v>78</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>221</v>
       </c>
@@ -1842,16 +1923,16 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" t="s">
-        <v>81</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>223</v>
       </c>
@@ -1859,16 +1940,19 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>226</v>
       </c>
@@ -1876,16 +1960,19 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" t="s">
         <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>227</v>
       </c>
@@ -1893,16 +1980,19 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
         <v>85</v>
-      </c>
-      <c r="D23" t="s">
-        <v>86</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>230</v>
       </c>
@@ -1910,16 +2000,16 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
         <v>87</v>
-      </c>
-      <c r="D24" t="s">
-        <v>88</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>253</v>
       </c>
@@ -1927,16 +2017,16 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
         <v>89</v>
-      </c>
-      <c r="D25" t="s">
-        <v>90</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>254</v>
       </c>
@@ -1944,16 +2034,19 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" t="s">
         <v>91</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>92</v>
       </c>
-      <c r="E26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>255</v>
       </c>
@@ -1961,16 +2054,16 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>256</v>
       </c>
@@ -1978,16 +2071,16 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" t="s">
         <v>95</v>
-      </c>
-      <c r="D28" t="s">
-        <v>96</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>257</v>
       </c>
@@ -1995,16 +2088,16 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" t="s">
         <v>97</v>
-      </c>
-      <c r="D29" t="s">
-        <v>98</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>258</v>
       </c>
@@ -2012,16 +2105,19 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
         <v>99</v>
       </c>
-      <c r="D30" t="s">
-        <v>100</v>
-      </c>
       <c r="E30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F30" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>264</v>
       </c>
@@ -2029,16 +2125,16 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" t="s">
         <v>101</v>
       </c>
-      <c r="D31" t="s">
-        <v>102</v>
-      </c>
       <c r="E31" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>300</v>
       </c>
@@ -2046,16 +2142,19 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>301</v>
       </c>
@@ -2063,16 +2162,16 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
         <v>104</v>
-      </c>
-      <c r="D33" t="s">
-        <v>105</v>
       </c>
       <c r="E33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>302</v>
       </c>
@@ -2080,16 +2179,16 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" t="s">
         <v>106</v>
-      </c>
-      <c r="D34" t="s">
-        <v>107</v>
       </c>
       <c r="E34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>303</v>
       </c>
@@ -2097,16 +2196,16 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
         <v>108</v>
-      </c>
-      <c r="D35" t="s">
-        <v>109</v>
       </c>
       <c r="E35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>305</v>
       </c>
@@ -2114,16 +2213,19 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" t="s">
         <v>110</v>
-      </c>
-      <c r="D36" t="s">
-        <v>111</v>
       </c>
       <c r="E36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>307</v>
       </c>
@@ -2131,16 +2233,16 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" t="s">
         <v>112</v>
-      </c>
-      <c r="D37" t="s">
-        <v>113</v>
       </c>
       <c r="E37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>308</v>
       </c>
@@ -2148,16 +2250,16 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
         <v>114</v>
-      </c>
-      <c r="D38" t="s">
-        <v>115</v>
       </c>
       <c r="E38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>309</v>
       </c>
@@ -2165,16 +2267,16 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" t="s">
         <v>116</v>
-      </c>
-      <c r="D39" t="s">
-        <v>117</v>
       </c>
       <c r="E39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>310</v>
       </c>
@@ -2182,16 +2284,16 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" t="s">
         <v>118</v>
-      </c>
-      <c r="D40" t="s">
-        <v>119</v>
       </c>
       <c r="E40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>312</v>
       </c>
@@ -2199,16 +2301,16 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" t="s">
         <v>120</v>
       </c>
-      <c r="D41" t="s">
-        <v>121</v>
-      </c>
       <c r="E41" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>313</v>
       </c>
@@ -2216,16 +2318,16 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" t="s">
         <v>122</v>
-      </c>
-      <c r="D42" t="s">
-        <v>123</v>
       </c>
       <c r="E42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>316</v>
       </c>
@@ -2233,16 +2335,16 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
         <v>124</v>
-      </c>
-      <c r="D43" t="s">
-        <v>125</v>
       </c>
       <c r="E43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>317</v>
       </c>
@@ -2250,16 +2352,16 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" t="s">
         <v>126</v>
-      </c>
-      <c r="D44" t="s">
-        <v>127</v>
       </c>
       <c r="E44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>318</v>
       </c>
@@ -2267,16 +2369,19 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" t="s">
         <v>129</v>
-      </c>
-      <c r="D45" t="s">
-        <v>130</v>
       </c>
       <c r="E45" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>320</v>
       </c>
@@ -2284,16 +2389,19 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>321</v>
       </c>
@@ -2301,16 +2409,19 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" t="s">
         <v>132</v>
-      </c>
-      <c r="D47" t="s">
-        <v>133</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>322</v>
       </c>
@@ -2318,16 +2429,19 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" t="s">
         <v>134</v>
-      </c>
-      <c r="D48" t="s">
-        <v>135</v>
       </c>
       <c r="E48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>323</v>
       </c>
@@ -2335,16 +2449,19 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" t="s">
         <v>136</v>
-      </c>
-      <c r="D49" t="s">
-        <v>137</v>
       </c>
       <c r="E49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>335</v>
       </c>
@@ -2352,16 +2469,16 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" t="s">
         <v>138</v>
-      </c>
-      <c r="D50" t="s">
-        <v>139</v>
       </c>
       <c r="E50" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>340</v>
       </c>
@@ -2369,16 +2486,16 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" t="s">
         <v>140</v>
-      </c>
-      <c r="D51" t="s">
-        <v>141</v>
       </c>
       <c r="E51" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>341</v>
       </c>
@@ -2386,16 +2503,16 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" t="s">
         <v>142</v>
-      </c>
-      <c r="D52" t="s">
-        <v>143</v>
       </c>
       <c r="E52" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>342</v>
       </c>
@@ -2403,16 +2520,16 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" t="s">
         <v>144</v>
-      </c>
-      <c r="D53" t="s">
-        <v>145</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>344</v>
       </c>
@@ -2420,16 +2537,16 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" t="s">
         <v>146</v>
-      </c>
-      <c r="D54" t="s">
-        <v>147</v>
       </c>
       <c r="E54" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>345</v>
       </c>
@@ -2437,16 +2554,16 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" t="s">
         <v>148</v>
-      </c>
-      <c r="D55" t="s">
-        <v>149</v>
       </c>
       <c r="E55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>358</v>
       </c>
@@ -2454,16 +2571,19 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" t="s">
+        <v>226</v>
+      </c>
+      <c r="E56" t="s">
         <v>150</v>
       </c>
-      <c r="D56" t="s">
-        <v>227</v>
-      </c>
-      <c r="E56" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>360</v>
       </c>
@@ -2471,16 +2591,19 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" t="s">
         <v>152</v>
-      </c>
-      <c r="D57" t="s">
-        <v>153</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>361</v>
       </c>
@@ -2488,16 +2611,16 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" t="s">
         <v>154</v>
-      </c>
-      <c r="D58" t="s">
-        <v>155</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>400</v>
       </c>
@@ -2505,16 +2628,16 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
+        <v>155</v>
+      </c>
+      <c r="D59" t="s">
         <v>156</v>
-      </c>
-      <c r="D59" t="s">
-        <v>157</v>
       </c>
       <c r="E59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>401</v>
       </c>
@@ -2522,16 +2645,19 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
+        <v>157</v>
+      </c>
+      <c r="D60" t="s">
         <v>158</v>
-      </c>
-      <c r="D60" t="s">
-        <v>159</v>
       </c>
       <c r="E60" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>402</v>
       </c>
@@ -2539,16 +2665,19 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
+        <v>159</v>
+      </c>
+      <c r="D61" t="s">
         <v>160</v>
-      </c>
-      <c r="D61" t="s">
-        <v>161</v>
       </c>
       <c r="E61" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>403</v>
       </c>
@@ -2556,16 +2685,16 @@
         <v>3</v>
       </c>
       <c r="C62" t="s">
+        <v>161</v>
+      </c>
+      <c r="D62" t="s">
         <v>162</v>
-      </c>
-      <c r="D62" t="s">
-        <v>163</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>404</v>
       </c>
@@ -2573,16 +2702,19 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D63" t="s">
         <v>164</v>
-      </c>
-      <c r="D63" t="s">
-        <v>165</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>405</v>
       </c>
@@ -2590,16 +2722,19 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
+        <v>165</v>
+      </c>
+      <c r="D64" t="s">
         <v>166</v>
-      </c>
-      <c r="D64" t="s">
-        <v>167</v>
       </c>
       <c r="E64" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>406</v>
       </c>
@@ -2607,16 +2742,19 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
+        <v>167</v>
+      </c>
+      <c r="D65" t="s">
         <v>168</v>
-      </c>
-      <c r="D65" t="s">
-        <v>169</v>
       </c>
       <c r="E65" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>412</v>
       </c>
@@ -2624,16 +2762,19 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
+        <v>169</v>
+      </c>
+      <c r="D66" t="s">
         <v>170</v>
-      </c>
-      <c r="D66" t="s">
-        <v>171</v>
       </c>
       <c r="E66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>414</v>
       </c>
@@ -2641,16 +2782,16 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
+        <v>171</v>
+      </c>
+      <c r="D67" t="s">
         <v>172</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>173</v>
       </c>
-      <c r="E67" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>418</v>
       </c>
@@ -2658,16 +2799,19 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" t="s">
         <v>175</v>
-      </c>
-      <c r="D68" t="s">
-        <v>176</v>
       </c>
       <c r="E68" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>419</v>
       </c>
@@ -2675,16 +2819,19 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
+        <v>176</v>
+      </c>
+      <c r="D69" t="s">
         <v>177</v>
-      </c>
-      <c r="D69" t="s">
-        <v>178</v>
       </c>
       <c r="E69" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>420</v>
       </c>
@@ -2692,16 +2839,19 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D70" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E70" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>421</v>
       </c>
@@ -2709,16 +2859,19 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E71" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>422</v>
       </c>
@@ -2726,16 +2879,19 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
+        <v>182</v>
+      </c>
+      <c r="D72" t="s">
         <v>183</v>
-      </c>
-      <c r="D72" t="s">
-        <v>184</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>423</v>
       </c>
@@ -2743,16 +2899,19 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
+        <v>184</v>
+      </c>
+      <c r="D73" t="s">
         <v>185</v>
-      </c>
-      <c r="D73" t="s">
-        <v>186</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>424</v>
       </c>
@@ -2760,16 +2919,19 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" t="s">
         <v>187</v>
-      </c>
-      <c r="D74" t="s">
-        <v>188</v>
       </c>
       <c r="E74" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>425</v>
       </c>
@@ -2777,16 +2939,19 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" t="s">
         <v>189</v>
-      </c>
-      <c r="D75" t="s">
-        <v>190</v>
       </c>
       <c r="E75" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>426</v>
       </c>
@@ -2794,16 +2959,19 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D76" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E76" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>427</v>
       </c>
@@ -2811,16 +2979,19 @@
         <v>3</v>
       </c>
       <c r="C77" t="s">
+        <v>191</v>
+      </c>
+      <c r="D77" t="s">
         <v>192</v>
-      </c>
-      <c r="D77" t="s">
-        <v>193</v>
       </c>
       <c r="E77" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>428</v>
       </c>
@@ -2828,16 +2999,16 @@
         <v>3</v>
       </c>
       <c r="C78" t="s">
+        <v>193</v>
+      </c>
+      <c r="D78" t="s">
         <v>194</v>
-      </c>
-      <c r="D78" t="s">
-        <v>195</v>
       </c>
       <c r="E78" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>437</v>
       </c>
@@ -2845,16 +3016,19 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
+        <v>196</v>
+      </c>
+      <c r="D79" t="s">
         <v>197</v>
-      </c>
-      <c r="D79" t="s">
-        <v>198</v>
       </c>
       <c r="E79" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>440</v>
       </c>
@@ -2862,16 +3036,19 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E80" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>441</v>
       </c>
@@ -2879,16 +3056,16 @@
         <v>3</v>
       </c>
       <c r="C81" t="s">
+        <v>199</v>
+      </c>
+      <c r="D81" t="s">
         <v>200</v>
-      </c>
-      <c r="D81" t="s">
-        <v>201</v>
       </c>
       <c r="E81" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>442</v>
       </c>
@@ -2896,16 +3073,16 @@
         <v>3</v>
       </c>
       <c r="C82" t="s">
+        <v>201</v>
+      </c>
+      <c r="D82" t="s">
         <v>202</v>
-      </c>
-      <c r="D82" t="s">
-        <v>203</v>
       </c>
       <c r="E82" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>443</v>
       </c>
@@ -2913,16 +3090,19 @@
         <v>3</v>
       </c>
       <c r="C83" t="s">
+        <v>203</v>
+      </c>
+      <c r="D83" t="s">
         <v>204</v>
-      </c>
-      <c r="D83" t="s">
-        <v>205</v>
       </c>
       <c r="E83" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>444</v>
       </c>
@@ -2930,16 +3110,16 @@
         <v>3</v>
       </c>
       <c r="C84" t="s">
+        <v>205</v>
+      </c>
+      <c r="D84" t="s">
         <v>206</v>
-      </c>
-      <c r="D84" t="s">
-        <v>207</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>446</v>
       </c>
@@ -2947,16 +3127,16 @@
         <v>3</v>
       </c>
       <c r="C85" t="s">
+        <v>207</v>
+      </c>
+      <c r="D85" t="s">
         <v>208</v>
-      </c>
-      <c r="D85" t="s">
-        <v>209</v>
       </c>
       <c r="E85" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>450</v>
       </c>
@@ -2964,16 +3144,19 @@
         <v>3</v>
       </c>
       <c r="C86" t="s">
+        <v>209</v>
+      </c>
+      <c r="D86" t="s">
         <v>210</v>
-      </c>
-      <c r="D86" t="s">
-        <v>211</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>462</v>
       </c>
@@ -2981,10 +3164,10 @@
         <v>3</v>
       </c>
       <c r="C87" t="s">
+        <v>211</v>
+      </c>
+      <c r="D87" t="s">
         <v>212</v>
-      </c>
-      <c r="D87" t="s">
-        <v>213</v>
       </c>
       <c r="E87" t="s">
         <v>7</v>
@@ -2999,7 +3182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DE2127-F1A0-9D43-BB22-8321377E9C1D}">
   <dimension ref="A1:I337"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
+    <sheetView topLeftCell="A295" workbookViewId="0">
       <selection activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
@@ -3036,10 +3219,10 @@
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -17237,10 +17420,10 @@
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -24430,10 +24613,10 @@
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -26364,7 +26547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA520945-B158-764D-823B-F47F242E4808}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="R39" activeCellId="1" sqref="C36 R39"/>
     </sheetView>
   </sheetViews>
@@ -27185,10 +27368,10 @@
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -29333,11 +29516,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC08885-D475-D740-B093-B1999F0EDA05}">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -29429,7 +29610,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -29443,7 +29624,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -29457,7 +29638,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -29471,7 +29652,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -29485,7 +29666,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -29499,7 +29680,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -29513,7 +29694,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -29527,7 +29708,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -29541,7 +29722,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -29555,7 +29736,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -29569,7 +29750,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -29583,7 +29764,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -29597,7 +29778,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -29611,7 +29792,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -29625,7 +29806,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -29639,7 +29820,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -29653,7 +29834,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -29681,7 +29862,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -29695,7 +29876,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -29709,7 +29890,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -29723,7 +29904,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -29737,7 +29918,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -29751,7 +29932,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -29765,7 +29946,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -29779,7 +29960,7 @@
         <v>14</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -29793,7 +29974,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -29821,7 +30002,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -29835,7 +30016,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -29849,7 +30030,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -29863,7 +30044,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -29877,7 +30058,7 @@
         <v>13</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -29891,7 +30072,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -29905,7 +30086,7 @@
         <v>13</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -29919,7 +30100,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -29933,7 +30114,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -29947,7 +30128,7 @@
         <v>13</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -29961,7 +30142,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -29975,7 +30156,7 @@
         <v>13</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -29989,7 +30170,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -30003,7 +30184,7 @@
         <v>14</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -30017,7 +30198,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -30031,7 +30212,7 @@
         <v>13</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -30045,7 +30226,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -30059,7 +30240,7 @@
         <v>13</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -30073,7 +30254,7 @@
         <v>13</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -30087,7 +30268,7 @@
         <v>13</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -30101,7 +30282,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -30115,7 +30296,7 @@
         <v>13</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -30129,7 +30310,7 @@
         <v>13</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -30143,7 +30324,7 @@
         <v>13</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -30157,7 +30338,7 @@
         <v>13</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -30171,7 +30352,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -30185,7 +30366,7 @@
         <v>13</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -30199,7 +30380,7 @@
         <v>14</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -30213,7 +30394,7 @@
         <v>13</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -30227,7 +30408,7 @@
         <v>13</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -30241,7 +30422,7 @@
         <v>13</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -30255,7 +30436,7 @@
         <v>13</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -30269,7 +30450,7 @@
         <v>13</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -30283,7 +30464,7 @@
         <v>13</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -30297,7 +30478,7 @@
         <v>13</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -30311,7 +30492,7 @@
         <v>13</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -30325,7 +30506,7 @@
         <v>13</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -30339,7 +30520,7 @@
         <v>13</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -30353,7 +30534,7 @@
         <v>13</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -30367,7 +30548,7 @@
         <v>13</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -30381,7 +30562,7 @@
         <v>13</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -30395,7 +30576,7 @@
         <v>13</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -30409,7 +30590,7 @@
         <v>13</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -30423,7 +30604,7 @@
         <v>13</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -30437,7 +30618,7 @@
         <v>13</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -30451,7 +30632,7 @@
         <v>13</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -30465,7 +30646,7 @@
         <v>14</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -30479,7 +30660,7 @@
         <v>13</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -30493,7 +30674,7 @@
         <v>13</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -30507,7 +30688,7 @@
         <v>13</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -30521,7 +30702,7 @@
         <v>13</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -30535,7 +30716,7 @@
         <v>13</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -30549,7 +30730,7 @@
         <v>13</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -30563,7 +30744,7 @@
         <v>13</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -30577,7 +30758,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -30591,7 +30772,7 @@
         <v>13</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -30605,7 +30786,7 @@
         <v>13</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -30619,7 +30800,7 @@
         <v>13</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -30633,7 +30814,7 @@
         <v>13</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -30647,7 +30828,7 @@
         <v>13</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -30661,7 +30842,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -30675,7 +30856,7 @@
         <v>13</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -30689,7 +30870,7 @@
         <v>13</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -30703,7 +30884,7 @@
         <v>13</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -30717,7 +30898,7 @@
         <v>13</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -30731,7 +30912,7 @@
         <v>13</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -30745,7 +30926,7 @@
         <v>14</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -30759,7 +30940,7 @@
         <v>14</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -30773,7 +30954,7 @@
         <v>13</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -30787,7 +30968,7 @@
         <v>13</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -30801,7 +30982,7 @@
         <v>13</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -30815,7 +30996,7 @@
         <v>13</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -30829,7 +31010,7 @@
         <v>13</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -30843,7 +31024,7 @@
         <v>13</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -30857,7 +31038,7 @@
         <v>13</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -30871,7 +31052,7 @@
         <v>13</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -30885,7 +31066,7 @@
         <v>13</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -30899,21 +31080,7 @@
         <v>13</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="4">
-        <v>125</v>
-      </c>
-      <c r="B112" s="4">
-        <v>404</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -30925,9 +31092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B521BB6-DE7E-F648-84B9-F67E5C6BF11B}">
   <dimension ref="A1:D337"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146:XFD146"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -30946,7 +31111,7 @@
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -35664,7 +35829,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36274,7 +36439,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36287,7 +36452,7 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -36295,7 +36460,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -36303,7 +36468,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -36311,7 +36476,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -36319,7 +36484,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -36327,7 +36492,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -36335,7 +36500,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -36343,7 +36508,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -36363,7 +36528,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -37045,7 +37210,7 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -37053,7 +37218,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -37061,7 +37226,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -37069,7 +37234,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -37077,7 +37242,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use UBC colors for highlighting. Remove advanced pure math tracks until we figure it out.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4410B1F-9B45-534D-A78C-D34BFC42C5C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A40C08-EF67-7046-8C89-5275EA97D0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="1060" windowWidth="25820" windowHeight="16400" firstSheet="8" activeTab="14" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="1600" yWindow="780" windowWidth="25820" windowHeight="16400" firstSheet="8" activeTab="14" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="377">
   <si>
     <t>number</t>
   </si>
@@ -1289,16 +1289,25 @@
     <t>Pure Mathematics: Discrete</t>
   </si>
   <si>
-    <t>Advanced Pure Mathematics: Algebra and Number Theory</t>
-  </si>
-  <si>
-    <t>Advanced Pure Mathematics: Algebra and Discrete Mathematics</t>
-  </si>
-  <si>
-    <t>Advanced Pure Mathematics: Algebra and Geometry</t>
-  </si>
-  <si>
-    <t>Advanced Pure Mathematics: Analysis</t>
+    <t>The &lt;a href="https://www.math.ubc.ca" target="_blank"&gt;UBC Department of Mathematics&lt;/a&gt; offers a wide range of undergraduate courses from calculus to number theory to mathematical biology. Explore the different &lt;a href="https://www.math.ubc.ca/undergraduate/programs-study" target="_blank"&gt;programs of study&lt;/a&gt; including BA/BSc Major in Mathematics, BA/BSc Honours in Mathematics, and courses offered for engineering programs.</t>
+  </si>
+  <si>
+    <t>The course map presents all MATH courses along with prerequisite/corequisite connections. Hover over a course to view the course description, a complete list of prerequisites/corequisites, credit exclusions and notes. Complete information is available in the &lt;a href="http://www.calendar.ubc.ca/vancouver/courses.cfm?page=name&amp;code=MATH" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt; and current course offerings are available in the &lt;a href="https://courses.students.ubc.ca/cs/courseschedule?pname=subjarea&amp;tname=subj-department&amp;dept=MATH" target="_blank"&gt;UBC Course Schedule&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Degree requirements for BA/BSc Major in Mathematics include:&lt;br&gt;&amp;bull; Calculus I (MATH 100, 102, 104, 180, 184, 110 or 120)&lt;br&gt;&amp;bull; Calculus II (MATH 101, 103, 105 or 121)&lt;br&gt;&amp;bull; Calculus III (MATH 200, 217 or 226)&lt;br&gt;&amp;bull; Mathematical Proof (MATH 220)&lt;br&gt;&amp;bull; Linear Algebra (MATH 221 or 223)&lt;br&gt;&amp;bull; Differential Equations (MATH 215)&lt;br&gt;&amp;bull; Mathematical Computing (MATH 210 or CPSC 210)&lt;br&gt;&amp;bull; 24 credits of MATH courses numbered 300 or above</t>
+  </si>
+  <si>
+    <t>After completing 100 and 200 level degree requirements, students in the BA/BSc Major in Mathematics program choose any 24 credits of MATH courses numbered 300 and above. Explore the different tracks within the program such as discrete mathematics and mathematical biology to find sequences of courses which work well together. Complete degree requirements are available in the &lt;a href="http://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,215,410,429" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Third and fourth year requirements include:&lt;br&gt;&amp;bull; MATH 300 Complex Analysis&lt;br&gt;&amp;bull; MATH 320 Real Variables I&lt;br&gt;&amp;bull; MATH 321 Real Variables II&lt;br&gt;&amp;bull; MATH 322 Introduction to Group Theory&lt;br&gt;&amp;bull; MATH 323 Introduction to Rings and Modules&lt;br&gt;&amp;bull; 15 credits from MATH 400-406, 412, 418-428, 433-440, 443, 449, 450&lt;br&gt;&amp;bull; Additional 9 credits of MATH courses numbered 300 or above</t>
+  </si>
+  <si>
+    <t>Degree requirements for BA/BSc Honours in Mathematics are listed in the &lt;a href="http://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,215,410,429" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt;. First and second year requirements are:&lt;br&gt;&amp;bull; Calculus I (MATH 100, 102, 104, 180, 184, 110 or 120)&lt;br&gt;&amp;bull; Calculus II (MATH 101, 103, 105 or 121)&lt;br&gt;&amp;bull; Calculus III (MATH 200, 217 or 226)&lt;br&gt;&amp;bull; Calculus IV (MATH 317 or 227)&lt;br&gt;&amp;bull; Linear Algebra (MATH 221 or 223)&lt;br&gt;&amp;bull; Differential Equations (MATH 215)&lt;br&gt;&amp;bull; Mathematical Computing (MATH 210 or CPSC 210)</t>
+  </si>
+  <si>
+    <t>Engineering courses are designed for specific applications and are reserved for APSC students.</t>
   </si>
 </sst>
 </file>
@@ -1363,12 +1372,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11172,10 +11184,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0A164B-708E-884A-B2CD-DB267B8D4A7F}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11354,16 +11366,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>370</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="A11" s="3">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E11" t="s">
@@ -11371,16 +11383,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>371</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="A12" s="3">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E12" t="s">
@@ -11388,16 +11400,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>372</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="A13" s="3">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E13" t="s">
@@ -11405,138 +11417,70 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>373</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="A14" s="3">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>321</v>
+        <v>226</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E17" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3">
-        <v>4</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>306</v>
       </c>
     </row>
@@ -11549,7 +11493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5605FB08-D761-1B4B-8F7E-F0D219ED9D4B}">
   <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A118" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -19416,7 +19360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC045EC-A8A3-974C-9403-34BA5D62B768}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
@@ -19874,11 +19818,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D05D007-E767-5440-814F-4CB4191763F7}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="4" width="75.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -19894,61 +19842,59 @@
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="C2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="C2" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="C3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="C3" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="C4" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C5" t="s">
-        <v>306</v>
-      </c>
-      <c r="D5" t="s">
-        <v>306</v>
-      </c>
+      <c r="C5" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add suggested STAT courses for Math of Data stream.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AEA852-07FD-E741-92F8-71B0CB9F64D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2506B917-5390-E640-8EC0-B3CEA4EAF303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="880" windowWidth="25820" windowHeight="16400" firstSheet="8" activeTab="14" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
@@ -1315,10 +1315,10 @@
     <t>This stream is centred on solving problems using numerical techniques and approximations. Topics in this stream have many applications in engineering, economics and computing. If you like solving math problems using software and programming, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 307, 316, 405, 340, 441, 360, 461&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 302, 303, 402, 406; PHYS 210, 410</t>
   </si>
   <si>
-    <t>This stream is centred on the theoretical foundations of data science. Topics in this stream have many applications in machine learning and signal processing. If you like algorithms and making sense of large data sets, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 307, 340, 441, 344 and 442&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 340, 440; PHIL 320, 321; PHYS 310</t>
-  </si>
-  <si>
     <t>This stream is centred on constructing and evaluating mathematical models. Topics in this stream have many applications in science, especially in mathematical biology and computational mathematics for physical problems. If you like multidisciplinary work and using mathematics to describe real-world problems, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 344, 345, 360+461 &lt;strong&gt;or&lt;/strong&gt; 361+462&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 330, 421; PHIL 321; PHYS 305</t>
+  </si>
+  <si>
+    <t>This stream is centred on the theoretical foundations of data science. Topics in this stream have many applications in machine learning and signal processing. If you like algorithms and making sense of large data sets, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 307, 340, 441, 344 and 442&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 340, 440; PHIL 320, 321; PHYS 310; STAT 301, 305, 306, 406</t>
   </si>
 </sst>
 </file>
@@ -11324,7 +11324,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11396,7 +11396,7 @@
         <v>363</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>357</v>
@@ -11413,7 +11413,7 @@
         <v>371</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>357</v>

</xml_diff>

<commit_message>
Edit track course lists.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D79341-7174-664F-BBC4-779D389663D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B740BEE-23DF-7B4C-983F-80A5D34A3695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="880" windowWidth="25820" windowHeight="16400" firstSheet="1" activeTab="6" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="1080" yWindow="880" windowWidth="25820" windowHeight="16400" firstSheet="9" activeTab="14" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -1303,22 +1303,22 @@
     <t>This stream is centred on classical problems in two of the most enduring branches of mathematics. Topics in this stream have modern applications in areas including cryptography and computer graphics. If you like patterns and puzzles, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 310, 341, 342, 308+309 &lt;strong&gt;or&lt;/strong&gt; 312+313&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 424; PHIL 320, 322, 323, 420</t>
   </si>
   <si>
-    <t>This stream is centred on the analysis of functions and the phenomena they describe, from quantum mechanics to celestial motion. Topics in this stream have many applications in physics and engineering. If you like calculus and want to learn about some of its most important applications, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 300, 301, 316, 400, 317, 319&lt;br&gt;&lt;br&gt;Suggested courses from other departments: PHYS 301, 304, 306</t>
-  </si>
-  <si>
-    <t>This stream is centred on solving problems using numerical techniques and approximations. Topics in this stream have many applications in engineering, economics and computing. If you like solving math problems using software and programming, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 307, 316, 405, 340, 441, 360, 461&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 302, 303, 402, 406; PHYS 210, 410</t>
-  </si>
-  <si>
     <t>This stream is centred on constructing and evaluating mathematical models. Topics in this stream have many applications in science, especially in mathematical biology and computational mathematics for physical problems. If you like multidisciplinary work and using mathematics to describe real-world problems, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 344, 345, 360+461 &lt;strong&gt;or&lt;/strong&gt; 361+462&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 330, 421; PHIL 321; PHYS 305</t>
   </si>
   <si>
-    <t>This stream is centred on the theoretical foundations of data science. Topics in this stream have many applications in machine learning and signal processing. If you like algorithms and making sense of large data sets, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 307, 340, 441, 344 and 442&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 340, 440; PHIL 320, 321; PHYS 310; STAT 301, 305, 306, 406</t>
-  </si>
-  <si>
     <t>Marvels of Mathematics</t>
   </si>
   <si>
     <t>A variety of topics in mathematics, showcasing its beauty and utility. Intended for a general audience of students whose degrees have no mathematics requirements, but who may be curious about practical and recreational mathematics. Not for credit in the Faculty of Science. Students who obtain UBC credit for any other mathematics course cannot in the same or later years obtain credit for MATH 230.</t>
+  </si>
+  <si>
+    <t>This stream is centred on the analysis of functions and the phenomena they describe, from quantum mechanics to celestial motion. Topics in this stream have many applications in physics and engineering. If you like calculus and want to learn about some of its most important applications, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 300, 301, 316, 317, 319, 400&lt;br&gt;&lt;br&gt;Suggested courses from other departments: PHYS 301, 304, 306</t>
+  </si>
+  <si>
+    <t>This stream is centred on solving problems using numerical techniques and approximations. Topics in this stream have many applications in engineering, economics and computing. If you like solving math problems using software and programming, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 307, 316, 340, 360, 405, 441, 461&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 302, 303, 402, 406; PHYS 210, 410</t>
+  </si>
+  <si>
+    <t>This stream is centred on the theoretical foundations of data science. Topics in this stream have many applications in machine learning and signal processing. If you like algorithms and making sense of large data sets, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 307, 340, 344, 441, 442&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 340, 440; PHIL 320, 321; PHYS 310; STAT 301, 305, 306, 406</t>
   </si>
 </sst>
 </file>
@@ -2198,10 +2198,10 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D24" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -11325,7 +11325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0A164B-708E-884A-B2CD-DB267B8D4A7F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -11364,7 +11364,7 @@
         <v>359</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>355</v>
@@ -11381,7 +11381,7 @@
         <v>360</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>355</v>
@@ -11398,7 +11398,7 @@
         <v>361</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>355</v>
@@ -11415,7 +11415,7 @@
         <v>369</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>355</v>
@@ -19422,7 +19422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D5E774-6755-684C-B2A6-0325506B6789}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New layout with student reflections
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B740BEE-23DF-7B4C-983F-80A5D34A3695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1571CBF9-0026-024F-96BB-5B188D19A694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="880" windowWidth="25820" windowHeight="16400" firstSheet="9" activeTab="14" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="920" yWindow="1200" windowWidth="27020" windowHeight="15820" firstSheet="4" activeTab="5" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="requisites_program4" sheetId="17" r:id="rId14"/>
     <sheet name="tracks" sheetId="4" r:id="rId15"/>
     <sheet name="courses_tracks" sheetId="9" r:id="rId16"/>
+    <sheet name="reflections" sheetId="19" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="LayoutRequisites" localSheetId="7">requisites_program1!$A$1:$G$189</definedName>
@@ -115,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="448">
   <si>
     <t>number</t>
   </si>
@@ -1102,27 +1103,12 @@
     <t>program_id</t>
   </si>
   <si>
-    <t>Mechanical Engineering</t>
-  </si>
-  <si>
-    <t>Engineering Physics</t>
-  </si>
-  <si>
     <t>description1</t>
   </si>
   <si>
     <t>description2</t>
   </si>
   <si>
-    <t>Manufacturing, Materials Engineering</t>
-  </si>
-  <si>
-    <t>Chemical, Civil, Environmental Engineering</t>
-  </si>
-  <si>
-    <t>Electrical, Computer Engineering</t>
-  </si>
-  <si>
     <t>Introduction to Real Analysis</t>
   </si>
   <si>
@@ -1249,21 +1235,6 @@
     <t>The &lt;a href="https://www.math.ubc.ca" target="_blank"&gt;UBC Department of Mathematics&lt;/a&gt; offers a wide range of undergraduate courses from calculus to number theory to mathematical biology. Explore the different &lt;a href="https://www.math.ubc.ca/undergraduate/programs-study" target="_blank"&gt;programs of study&lt;/a&gt; including BA/BSc Major in Mathematics, BA/BSc Honours in Mathematics, and courses offered for engineering programs.</t>
   </si>
   <si>
-    <t>The course map presents all MATH courses along with prerequisite/corequisite connections. Hover over a course to view the course description, a complete list of prerequisites/corequisites, credit exclusions and notes. Complete information is available in the &lt;a href="http://www.calendar.ubc.ca/vancouver/courses.cfm?page=name&amp;code=MATH" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt; and current course offerings are available in the &lt;a href="https://courses.students.ubc.ca/cs/courseschedule?pname=subjarea&amp;tname=subj-department&amp;dept=MATH" target="_blank"&gt;UBC Course Schedule&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Degree requirements for BA/BSc Major in Mathematics include:&lt;br&gt;&amp;bull; Calculus I (MATH 100, 102, 104, 180, 184, 110 or 120)&lt;br&gt;&amp;bull; Calculus II (MATH 101, 103, 105 or 121)&lt;br&gt;&amp;bull; Calculus III (MATH 200, 217 or 226)&lt;br&gt;&amp;bull; Mathematical Proof (MATH 220)&lt;br&gt;&amp;bull; Linear Algebra (MATH 221 or 223)&lt;br&gt;&amp;bull; Differential Equations (MATH 215)&lt;br&gt;&amp;bull; Mathematical Computing (MATH 210 or CPSC 210)&lt;br&gt;&amp;bull; 24 credits of MATH courses numbered 300 or above</t>
-  </si>
-  <si>
-    <t>Third and fourth year requirements include:&lt;br&gt;&amp;bull; MATH 300 Complex Analysis&lt;br&gt;&amp;bull; MATH 320 Real Variables I&lt;br&gt;&amp;bull; MATH 321 Real Variables II&lt;br&gt;&amp;bull; MATH 322 Introduction to Group Theory&lt;br&gt;&amp;bull; MATH 323 Introduction to Rings and Modules&lt;br&gt;&amp;bull; 15 credits from MATH 400-406, 412, 418-428, 433-440, 443, 449, 450&lt;br&gt;&amp;bull; Additional 9 credits of MATH courses numbered 300 or above</t>
-  </si>
-  <si>
-    <t>Degree requirements for BA/BSc Honours in Mathematics are listed in the &lt;a href="http://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,215,410,429" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt;. First and second year requirements are:&lt;br&gt;&amp;bull; Calculus I (MATH 100, 102, 104, 180, 184, 110 or 120)&lt;br&gt;&amp;bull; Calculus II (MATH 101, 103, 105 or 121)&lt;br&gt;&amp;bull; Calculus III (MATH 200, 217 or 226)&lt;br&gt;&amp;bull; Calculus IV (MATH 317 or 227)&lt;br&gt;&amp;bull; Linear Algebra (MATH 221 or 223)&lt;br&gt;&amp;bull; Differential Equations (MATH 215)&lt;br&gt;&amp;bull; Mathematical Computing (MATH 210 or CPSC 210)</t>
-  </si>
-  <si>
-    <t>Engineering courses are designed for specific applications and are reserved for APSC students.</t>
-  </si>
-  <si>
     <t>Differential Equations and Analysis</t>
   </si>
   <si>
@@ -1300,25 +1271,265 @@
     <t>After completing 100 and 200 level degree requirements, students in the BA/BSc Major in Mathematics program choose any 24 credits of MATH courses numbered 300 and above. Certain courses work especially well together. Math majors are strongly recommended to select all the courses in one of the five listed streams. Complete degree requirements are available in the &lt;a href="http://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,215,410,429" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt;.</t>
   </si>
   <si>
-    <t>This stream is centred on classical problems in two of the most enduring branches of mathematics. Topics in this stream have modern applications in areas including cryptography and computer graphics. If you like patterns and puzzles, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 310, 341, 342, 308+309 &lt;strong&gt;or&lt;/strong&gt; 312+313&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 424; PHIL 320, 322, 323, 420</t>
-  </si>
-  <si>
-    <t>This stream is centred on constructing and evaluating mathematical models. Topics in this stream have many applications in science, especially in mathematical biology and computational mathematics for physical problems. If you like multidisciplinary work and using mathematics to describe real-world problems, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 344, 345, 360+461 &lt;strong&gt;or&lt;/strong&gt; 361+462&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 330, 421; PHIL 321; PHYS 305</t>
-  </si>
-  <si>
     <t>Marvels of Mathematics</t>
   </si>
   <si>
     <t>A variety of topics in mathematics, showcasing its beauty and utility. Intended for a general audience of students whose degrees have no mathematics requirements, but who may be curious about practical and recreational mathematics. Not for credit in the Faculty of Science. Students who obtain UBC credit for any other mathematics course cannot in the same or later years obtain credit for MATH 230.</t>
   </si>
   <si>
-    <t>This stream is centred on the analysis of functions and the phenomena they describe, from quantum mechanics to celestial motion. Topics in this stream have many applications in physics and engineering. If you like calculus and want to learn about some of its most important applications, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 300, 301, 316, 317, 319, 400&lt;br&gt;&lt;br&gt;Suggested courses from other departments: PHYS 301, 304, 306</t>
-  </si>
-  <si>
-    <t>This stream is centred on solving problems using numerical techniques and approximations. Topics in this stream have many applications in engineering, economics and computing. If you like solving math problems using software and programming, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 307, 316, 340, 360, 405, 441, 461&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 302, 303, 402, 406; PHYS 210, 410</t>
-  </si>
-  <si>
-    <t>This stream is centred on the theoretical foundations of data science. Topics in this stream have many applications in machine learning and signal processing. If you like algorithms and making sense of large data sets, this stream is for you.&lt;br&gt;&lt;br&gt;Courses: MATH 302, 303, 307, 340, 344, 441, 442&lt;br&gt;&lt;br&gt;Suggested courses from other departments: CPSC 340, 440; PHIL 320, 321; PHYS 310; STAT 301, 305, 306, 406</t>
+    <t>reflection_id</t>
+  </si>
+  <si>
+    <t>currently</t>
+  </si>
+  <si>
+    <t>James Yu</t>
+  </si>
+  <si>
+    <t>PhD Student in Economics</t>
+  </si>
+  <si>
+    <t>UBC Math and Economics 2022</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>MATH 302, 307, 340, 442</t>
+  </si>
+  <si>
+    <t>Many everyday optimization problems can be solved through the lens of graph-analyzing algorithms.</t>
+  </si>
+  <si>
+    <t>quote</t>
+  </si>
+  <si>
+    <t>reflection</t>
+  </si>
+  <si>
+    <t>I took Math 442 (Graphs and Networks) to formalize my interest in studying networks, an area I now explore in studying game theory as a PhD student in Economics. My biggest takeaway from the course was the idea that many everyday optimization problems can be solved through the lens of graph-analyzing algorithms: pathfinding, scheduling, searching and more. I learned that by representing a problem as a graph of vertices and edges, we give structure to difficult, high-dimensional scenarios. These structures then allow us to efficiently solve problems via algorithmic analysis, unlocking improvements in our lives that were previously inaccessible. In my research and graduate studies, I now use many of these models to gain insight into the welfare of individuals interacting in network environments such as markets and social media. By modeling these environments with graphs, we can determine if there are opportunities for systemic change, which can lead to beneficial welfare improvements in the lives of these individuals.</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Degree requirements for BA/BSc Major in Mathematics include:&lt;ul&gt;&lt;li&gt;Calculus I (MATH 100, 102, 104, 180, 184, 110 or 120)&lt;/li&gt;&lt;li&gt;Calculus II (MATH 101, 103, 105 or 121)&lt;/li&gt;&lt;li&gt;Calculus III (MATH 200, 217 or 226)&lt;/li&gt;&lt;li&gt;Mathematical Proof (MATH 220)&lt;/li&gt;&lt;li&gt;Linear Algebra (MATH 221 or 223)&lt;/li&gt;&lt;li&gt;Differential Equations (MATH 215)&lt;/li&gt;&lt;li&gt;Mathematical Computing (MATH 210 or CPSC 210)&lt;/li&gt;&lt;li&gt;24 credits of MATH courses numbered 300 or above&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>suggested</t>
+  </si>
+  <si>
+    <t>MATH 300, 301, 316, 317, 319, 400</t>
+  </si>
+  <si>
+    <t>This stream is centred on the analysis of functions and the phenomena they describe, from quantum mechanics to celestial motion. Topics in this stream have many applications in physics and engineering. If you like calculus and want to learn about some of its most important applications, this stream is for you.</t>
+  </si>
+  <si>
+    <t>PHYS 301, 304, 306</t>
+  </si>
+  <si>
+    <t>MATH 307, 316, 340, 360, 405, 441, 461</t>
+  </si>
+  <si>
+    <t>This stream is centred on solving problems using numerical techniques and approximations. Topics in this stream have many applications in engineering, economics and computing. If you like solving math problems using software and programming, this stream is for you.</t>
+  </si>
+  <si>
+    <t>CPSC 302, 303, 402, 406; PHYS 210, 410</t>
+  </si>
+  <si>
+    <t>MATH 302, 303, 307, 340, 344, 441, 442</t>
+  </si>
+  <si>
+    <t>This stream is centred on the theoretical foundations of data science. Topics in this stream have many applications in machine learning and signal processing. If you like algorithms and making sense of large data sets, this stream is for you.</t>
+  </si>
+  <si>
+    <t>CPSC 340, 440; PHIL 320, 321; PHYS 310; STAT 301, 305, 306, 406</t>
+  </si>
+  <si>
+    <t>MATH 302, 303, 344, 345, 360+461 &lt;strong&gt;or&lt;/strong&gt; 361+462</t>
+  </si>
+  <si>
+    <t>This stream is centred on constructing and evaluating mathematical models. Topics in this stream have many applications in science, especially in mathematical biology and computational mathematics for physical problems. If you like multidisciplinary work and using mathematics to describe real-world problems, this stream is for you.</t>
+  </si>
+  <si>
+    <t>CPSC 330, 421; PHIL 321; PHYS 305</t>
+  </si>
+  <si>
+    <t>MATH 310, 341, 342, 308+309 &lt;strong&gt;or&lt;/strong&gt; 312+313</t>
+  </si>
+  <si>
+    <t>This stream is centred on classical problems in two of the most enduring branches of mathematics. Topics in this stream have modern applications in areas including cryptography and computer graphics. If you like patterns and puzzles, this stream is for you.</t>
+  </si>
+  <si>
+    <t>CPSC 424; PHIL 320, 322, 323, 420</t>
+  </si>
+  <si>
+    <t>Complete information is available in the &lt;a href="http://www.calendar.ubc.ca/vancouver/courses.cfm?page=name&amp;code=MATH" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt; and current course offerings are available in the &lt;a href="https://courses.students.ubc.ca/cs/courseschedule?pname=subjarea&amp;tname=subj-department&amp;dept=MATH" target="_blank"&gt;UBC Course Schedule&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Degree requirements for BA/BSc Honours in Mathematics are listed in the &lt;a href="http://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,215,410,429" target="_blank"&gt;UBC Academic Calendar&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>First and second year requirements are:&lt;ul&gt;&lt;li&gt;Calculus I (MATH 100, 102, 104, 180, 184, 110 or 120)&lt;/li&gt;&lt;li&gt;Calculus II (MATH 101, 103, 105 or 121)&lt;/li&gt;&lt;li&gt;Calculus III (MATH 200, 217 or 226)&lt;/li&gt;&lt;li&gt;Calculus IV (MATH 317 or 227)&lt;/li&gt;&lt;li&gt;Linear Algebra (MATH 221 or 223)&lt;/li&gt;&lt;li&gt;Differential Equations (MATH 215)&lt;/li&gt;&lt;li&gt;Mathematical Computing (MATH 210 or CPSC 210)&lt;/li&gt;&lt;/ul&gt;Third and fourth year requirements include:&lt;ul&gt;&lt;li&gt;MATH 300 Complex Analysis&lt;/li&gt;&lt;li&gt;MATH 320 Real Variables I&lt;/li&gt;&lt;li&gt;MATH 321 Real Variables II&lt;/li&gt;&lt;li&gt;MATH 322 Introduction to Group Theory&lt;/li&gt;&lt;li&gt;MATH 323 Introduction to Rings and Modules&lt;/li&gt;&lt;li&gt;15 credits from MATH 400-406, 412, 418-428, 433-440, 443, 449, 450&lt;/li&gt;&lt;li&gt;Additional 9 credits of MATH courses numbered 300 or above&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Fiona Sudihok</t>
+  </si>
+  <si>
+    <t>Systems Engineer</t>
+  </si>
+  <si>
+    <t>UBC Math 2020</t>
+  </si>
+  <si>
+    <t>Math courses are not easy and fairly rigorous, and I think that having gone through them during undergrad in general made me a better problem solver, which is a very crucial skill in my day to day work. I really enjoyed a lot of the courses I took while I was in the program, but if I could change things up I would have liked to take courses that are more connected to each other to gain deeper knowledge on certain topics, as opposed to taking a more "introductory" course at every level.</t>
+  </si>
+  <si>
+    <t>Jingyuan Hu</t>
+  </si>
+  <si>
+    <t>PhD Student in Operations Research</t>
+  </si>
+  <si>
+    <t>UBC Math 2019</t>
+  </si>
+  <si>
+    <t>MATH 300, 302, 317</t>
+  </si>
+  <si>
+    <t>My thorough training in analysis and probability has proved immensely valuable.</t>
+  </si>
+  <si>
+    <t>As a PhD student in Operations Research, I frequently grapple with problems related to optimization and machine learning, and my thorough training in analysis and probability has proved immensely valuable. Whether you're engaged in research or an internship, acquiring knowledge in advanced courses sooner rather than later will give you a competitive edge. After all, the earlier you start, the more margin for error you have. Talk to your teachers and classmates often – having diverse perspectives and ideas is always beneficial.</t>
+  </si>
+  <si>
+    <t>JingyuanHu.jpg</t>
+  </si>
+  <si>
+    <t>MSc Student in Astrophysics</t>
+  </si>
+  <si>
+    <t>Megan Oxland</t>
+  </si>
+  <si>
+    <t>MATH 300, 301, 316, 317, 400</t>
+  </si>
+  <si>
+    <t>The math courses that were heavily focused on linear algebra, calculus, and differential equations turned out to be the most useful.</t>
+  </si>
+  <si>
+    <t>The math courses I took at UBC allowed me to explore my passions and taught me the foundational problem-solving skills I still use on a daily basis. I learned early on I was much more interested in applied math, yet every course I took still turned out to be valuable. In my day-to-day work in Astrophysics, the math courses that were heavily focused on linear algebra, calculus, and differential equations turned out to be the most useful. If you like MATH 316, MATH 400 is a natural continuation. And in MATH 317 the vector operators (i.e. gradient, divergence, curl, etc.) and theorems (i.e. Gauss, Stokes etc.) are extremely important topics that always arise in physics.&lt;br&gt;&lt;br&gt;There are a large number of electives Math students are able to take. Take the opportunity to select courses that are of interest, and not just ones that your friends are taking or are known to boost your average. This is the time to learn about all disciplines, and if you find something you are truly passionate about, stick with it and consider adding a minor to your degree. No only will you enjoy your electives, but a minor will organize your electives in a logical way and may provide you with future opportunities. One final piece of advice: go to office hours! I cannot stress this enough. Your professors are there to help you, and although it may be intimidating at first you will always feel much better after leaving.</t>
+  </si>
+  <si>
+    <t>Shuwen Jiang</t>
+  </si>
+  <si>
+    <t>MSc in Finance</t>
+  </si>
+  <si>
+    <t>UBC Math and Economics 2021</t>
+  </si>
+  <si>
+    <t>MATH 307, 316, 340</t>
+  </si>
+  <si>
+    <t>MATH 340 (Introduction to Linear Programming) taught me how to think about optimization problems, such as how to maximize profit with constraints on risk.</t>
+  </si>
+  <si>
+    <t>JamesYu.png</t>
+  </si>
+  <si>
+    <t>Faner Chen</t>
+  </si>
+  <si>
+    <t>FanerChen.jpg</t>
+  </si>
+  <si>
+    <t>Investment Banker</t>
+  </si>
+  <si>
+    <t>MATH 302, 345, 360</t>
+  </si>
+  <si>
+    <t>Every time I encounter big problems, I always try to break them into smaller ones and approach them step by step.</t>
+  </si>
+  <si>
+    <t>I might not remember every single theorem I learned in class, but what I value most is the skill of problem solving and logical thinking. During my first two years at UBC, I always wondered how I can apply what I have learned to something practical. Then I took some courses in mathematical modelling, like MATH 345 and MATH 360. In these courses, some real-world problems were seemingly impossible to solve. We were expected to break them down into smaller pieces and make reasonable assumptions. In my job, every time I encounter big problems, I always try to break them into smaller ones and approach them step by step.</t>
+  </si>
+  <si>
+    <t>Chuxuan Zhang</t>
+  </si>
+  <si>
+    <t>ChuxuanZhang.jpg</t>
+  </si>
+  <si>
+    <t>MSc Student in Computer Science</t>
+  </si>
+  <si>
+    <t>UBC Math 2022</t>
+  </si>
+  <si>
+    <t>MATH 302, 303, 361</t>
+  </si>
+  <si>
+    <t>You can learn classical biological models and get inspired by them even if your research interest seems in a completely different domain.</t>
+  </si>
+  <si>
+    <t>MATH 361 helped me gain a lot of insight. I'm now doing research in the area of affective computing where I refine existing models which predict/classify human emotions. It is intuitive and straightforward to draw analogies between human emotions and biological systems. As humans, we experience complex emotions instead of monotone discrete emotions at any time. For example, if you are into horror movies, you probably have the combined feeling of being scared and thrilled when watching them. But too much fear might kill your joy, and too much joy won’t give you a sense of dread at all. The dynamic equilibrium is similar to the classical Lotka-Volterra predator-prey model which is taught in MATH 361! MATH 361 is a course where you can learn classical biological models and get inspired by them even if your research interest seems in a completely different domain.</t>
+  </si>
+  <si>
+    <t>Joshua Renault</t>
+  </si>
+  <si>
+    <t>JoshuaRenault.png</t>
+  </si>
+  <si>
+    <t>MSc Student in Math</t>
+  </si>
+  <si>
+    <t>MATH 310, 312, 313</t>
+  </si>
+  <si>
+    <t>If you allow yourself to be amazed by the discipline, you will excel.</t>
+  </si>
+  <si>
+    <t>The abstract nature of MATH 313 (Topics in Number Theory) is fascinating. I believe that this course gave me the skills to be confident starting any proof. This course will definitely have you closing your eyes and trying to imagine different spaces, and it is totally worth it.  (Take MATH 312 not STAT 312 as a prerequisite. It’s tougher but what you learn doing the proofs is invaluable.)&lt;br&gt;&lt;br&gt;I think the best advice I can offer is to enjoy the math you are taking. It is definitely a challenging degree, but if you allow yourself to be amazed by the discipline, you will excel.</t>
+  </si>
+  <si>
+    <t>Karishma Sharma</t>
+  </si>
+  <si>
+    <t>High School Math Teacher</t>
+  </si>
+  <si>
+    <t>MATH 308, 310, 312, 342</t>
+  </si>
+  <si>
+    <t>MATH 308 is where I really began to develop a love of proofs.</t>
+  </si>
+  <si>
+    <t>MATH 308 is where I really began to develop a love of proofs. It was the first time I really understood how to approach proofs and how much fun they could be. This later directly applied to my job as I taught Foundations of Math 11/12 during my Teacher Education Practicum and had to be familiar with geometry proofs in particular. I learned relevant math teaching skills from this course as well. The way it was designed allowed us to problem-solve in less traditional ways. Assignments were formatted in a way that promoted student learning, so now I am able to apply those same strategies when assigning work to students. The prof I had for this course helped inspire me to dig deeper with my learning by asking guiding questions, and also engaging in teaching strategy discussions during office hours, which again has influenced my current teaching practices. I will be forever grateful for this course and the prof I had for inspiring and empowering me in so many different ways.</t>
+  </si>
+  <si>
+    <t>MeganOxland.jpeg</t>
+  </si>
+  <si>
+    <t>KarishmaSharma.jpg</t>
+  </si>
+  <si>
+    <t>ShuwenJiang.jpg</t>
+  </si>
+  <si>
+    <t>Math courses are not easy and fairly rigorous, and I think that having gone through them during undergrad in general made me a better problem solver.</t>
+  </si>
+  <si>
+    <t>ubc.png</t>
+  </si>
+  <si>
+    <t>Engineering courses are designed for specific applications and are usually reserved for APSC students.</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1396,6 +1607,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1776,7 +1990,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1796,7 +2010,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1816,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1836,7 +2050,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1856,7 +2070,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1876,7 +2090,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1896,7 +2110,7 @@
         <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1916,7 +2130,7 @@
         <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1936,7 +2150,7 @@
         <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1956,7 +2170,7 @@
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1976,7 +2190,7 @@
         <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1996,7 +2210,7 @@
         <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2033,7 +2247,7 @@
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2070,7 +2284,7 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2090,7 +2304,7 @@
         <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2127,7 +2341,7 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2147,7 +2361,7 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2167,7 +2381,7 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2198,10 +2412,10 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="D24" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -2224,7 +2438,7 @@
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2244,7 +2458,7 @@
         <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2264,7 +2478,7 @@
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2284,7 +2498,7 @@
         <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2304,7 +2518,7 @@
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2324,7 +2538,7 @@
         <v>89</v>
       </c>
       <c r="F30" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2344,7 +2558,7 @@
         <v>277</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2401,7 +2615,7 @@
         <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2421,7 +2635,7 @@
         <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2512,7 +2726,7 @@
         <v>7</v>
       </c>
       <c r="F40" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2572,7 +2786,7 @@
         <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2592,7 +2806,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2612,7 +2826,7 @@
         <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2623,16 +2837,16 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D46" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E46" t="s">
         <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2652,7 +2866,7 @@
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2834,7 +3048,7 @@
         <v>147</v>
       </c>
       <c r="F57" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2845,10 +3059,10 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="D58" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
@@ -3003,7 +3217,7 @@
         <v>7</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -3260,7 +3474,7 @@
         <v>7</v>
       </c>
       <c r="F79" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -3416,10 +3630,10 @@
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="D88" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="E88" t="s">
         <v>7</v>
@@ -5947,7 +6161,7 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -8743,7 +8957,7 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -9174,7 +9388,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11323,20 +11537,20 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0A164B-708E-884A-B2CD-DB267B8D4A7F}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
-    <col min="4" max="4" width="62.83203125" customWidth="1"/>
-    <col min="5" max="5" width="75" customWidth="1"/>
+    <col min="3" max="5" width="32.83203125" customWidth="1"/>
+    <col min="6" max="6" width="62.83203125" customWidth="1"/>
+    <col min="7" max="7" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -11347,13 +11561,19 @@
         <v>278</v>
       </c>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>369</v>
       </c>
       <c r="E1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="116" customHeight="1" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="F1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="116" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -11361,16 +11581,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -11378,16 +11604,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -11395,16 +11627,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -11412,16 +11650,22 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -11429,89 +11673,20 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>352</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>376</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11520,7 +11695,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5605FB08-D761-1B4B-8F7E-F0D219ED9D4B}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11814,284 +11989,346 @@
         <v>313</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>10</v>
-      </c>
-      <c r="B37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>10</v>
-      </c>
-      <c r="B38">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>10</v>
-      </c>
-      <c r="B39">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>10</v>
-      </c>
-      <c r="B40">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>10</v>
-      </c>
-      <c r="B41">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>10</v>
-      </c>
-      <c r="B42">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>13</v>
-      </c>
-      <c r="B43">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>13</v>
-      </c>
-      <c r="B44">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>13</v>
-      </c>
-      <c r="B45">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>13</v>
-      </c>
-      <c r="B46">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>13</v>
-      </c>
-      <c r="B47">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>14</v>
-      </c>
-      <c r="B48">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>14</v>
-      </c>
-      <c r="B49">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>14</v>
-      </c>
-      <c r="B50">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>14</v>
-      </c>
-      <c r="B51">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>14</v>
-      </c>
-      <c r="B52">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>11</v>
-      </c>
-      <c r="B53">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>11</v>
-      </c>
-      <c r="B54">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>11</v>
-      </c>
-      <c r="B55">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>11</v>
-      </c>
-      <c r="B56">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>11</v>
-      </c>
-      <c r="B57">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>11</v>
-      </c>
-      <c r="B58">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>12</v>
-      </c>
-      <c r="B59">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>12</v>
-      </c>
-      <c r="B60">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>12</v>
-      </c>
-      <c r="B61">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>12</v>
-      </c>
-      <c r="B62">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>12</v>
-      </c>
-      <c r="B63">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>12</v>
-      </c>
-      <c r="B64">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>12</v>
-      </c>
-      <c r="B65">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>12</v>
-      </c>
-      <c r="B66">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>12</v>
-      </c>
-      <c r="B67">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>12</v>
-      </c>
-      <c r="B68">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE88373-DABB-E24C-8F06-14D0F52FB5C0}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="12.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="23" style="7" customWidth="1"/>
+    <col min="6" max="7" width="29.1640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="74.6640625" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>12</v>
-      </c>
-      <c r="B69">
+      <c r="F2" s="7" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>12</v>
-      </c>
-      <c r="B70">
+      <c r="G2" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>12</v>
-      </c>
-      <c r="B71">
-        <v>406</v>
+    <row r="3" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="136" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="289" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="204" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -12977,7 +13214,7 @@
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -13705,7 +13942,7 @@
         <v>12</v>
       </c>
       <c r="D114" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -13747,7 +13984,7 @@
         <v>12</v>
       </c>
       <c r="D117" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -18869,7 +19106,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -19337,7 +19574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D05D007-E767-5440-814F-4CB4191763F7}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19353,10 +19592,10 @@
         <v>278</v>
       </c>
       <c r="C1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
@@ -19367,10 +19606,10 @@
         <v>279</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>354</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
@@ -19381,10 +19620,10 @@
         <v>300</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
@@ -19395,10 +19634,10 @@
         <v>299</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>356</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
@@ -19409,7 +19648,7 @@
         <v>301</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>358</v>
+        <v>447</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -19450,7 +19689,7 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -34790,7 +35029,7 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Set minimum height of program info grid element
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1571CBF9-0026-024F-96BB-5B188D19A694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64A6261-EB4A-8648-84D0-1C97275972C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1200" windowWidth="27020" windowHeight="15820" firstSheet="4" activeTab="5" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="920" yWindow="1200" windowWidth="27020" windowHeight="15820" firstSheet="3" activeTab="5" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="449">
   <si>
     <t>number</t>
   </si>
@@ -1530,6 +1530,25 @@
   </si>
   <si>
     <t>Engineering courses are designed for specific applications and are usually reserved for APSC students.</t>
+  </si>
+  <si>
+    <t>Courses in &lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,33"&gt;Bachelor of Applied Science&lt;/a&gt; programs include:
+&lt;ul&gt;
+&lt;li&gt;All programs: MATH 100, 101, 152&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,1612"&gt;Biomedical Engineering (BMEG)&lt;/a&gt;: MATH 253, 256, 264&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,35"&gt;Chemical and Biological Engineering (CHBE)&lt;/a&gt;: MATH 253, 256&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,37"&gt;Civil Engineering (CIVL)&lt;/a&gt;: MATH 253, 256&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,39"&gt;Electrical Engineering (ELEC)&lt;/a&gt;: MATH 253, 256, 264&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,39"&gt;Computer Engineering (ELEC)&lt;/a&gt;: MATH 220, 253, 256, 318&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,40"&gt;Engineering Physics (ENPH)&lt;/a&gt;: MATH 217, 255, 257, 305, 307, 318, 400, 401, 405, 406&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,1679"&gt;Environmental Engineering (ENVE)&lt;/a&gt;: MATH 253, 256&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,41"&gt;Geological Engineering&lt;/a&gt;: MATH 253&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,42"&gt;Integrated Engineering (IGEN)&lt;/a&gt;: MATH 253, 255&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,1665"&gt;Manufacturing Engineering (MANU)&lt;/a&gt;: MATH 253, 255&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,44"&gt;Materials Engineering (MTRL)&lt;/a&gt;: MATH 253, 255&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,43"&gt;Mechanical Engineering (MECH)&lt;/a&gt;: MATH 254, 258, 358&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,45"&gt;Mining Engineering (MINE)&lt;/a&gt;: MATH 253, 255&lt;/li&gt;
+&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -11999,7 +12018,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12107,7 +12126,7 @@
         <v>416</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>277</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="221" x14ac:dyDescent="0.2">
@@ -19650,7 +19669,9 @@
       <c r="C5" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update courses in streams
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickwalls/Documents/work/uper/coursemap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64A6261-EB4A-8648-84D0-1C97275972C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75638E36-F54E-EF41-A635-5B0B5D1BE6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1200" windowWidth="27020" windowHeight="15820" firstSheet="3" activeTab="5" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
+    <workbookView xWindow="920" yWindow="1200" windowWidth="27020" windowHeight="15820" firstSheet="8" activeTab="15" xr2:uid="{51EE6A31-502D-6549-9177-715EB70CBFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -1322,9 +1322,6 @@
     <t>suggested</t>
   </si>
   <si>
-    <t>MATH 300, 301, 316, 317, 319, 400</t>
-  </si>
-  <si>
     <t>This stream is centred on the analysis of functions and the phenomena they describe, from quantum mechanics to celestial motion. Topics in this stream have many applications in physics and engineering. If you like calculus and want to learn about some of its most important applications, this stream is for you.</t>
   </si>
   <si>
@@ -1349,16 +1346,10 @@
     <t>CPSC 340, 440; PHIL 320, 321; PHYS 310; STAT 301, 305, 306, 406</t>
   </si>
   <si>
-    <t>MATH 302, 303, 344, 345, 360+461 &lt;strong&gt;or&lt;/strong&gt; 361+462</t>
-  </si>
-  <si>
     <t>This stream is centred on constructing and evaluating mathematical models. Topics in this stream have many applications in science, especially in mathematical biology and computational mathematics for physical problems. If you like multidisciplinary work and using mathematics to describe real-world problems, this stream is for you.</t>
   </si>
   <si>
     <t>CPSC 330, 421; PHIL 321; PHYS 305</t>
-  </si>
-  <si>
-    <t>MATH 310, 341, 342, 308+309 &lt;strong&gt;or&lt;/strong&gt; 312+313</t>
   </si>
   <si>
     <t>This stream is centred on classical problems in two of the most enduring branches of mathematics. Topics in this stream have modern applications in areas including cryptography and computer graphics. If you like patterns and puzzles, this stream is for you.</t>
@@ -1549,6 +1540,15 @@
 &lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,43"&gt;Mechanical Engineering (MECH)&lt;/a&gt;: MATH 254, 258, 358&lt;/li&gt;
 &lt;li&gt;&lt;a href="https://www.calendar.ubc.ca/vancouver/index.cfm?tree=12,195,272,45"&gt;Mining Engineering (MINE)&lt;/a&gt;: MATH 253, 255&lt;/li&gt;
 &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>MATH 300, 301, 316, 317, 319, 400, 405</t>
+  </si>
+  <si>
+    <t>MATH 302, 303, 316, 344, 345, 360+461 &lt;strong&gt;or&lt;/strong&gt; 361+462</t>
+  </si>
+  <si>
+    <t>MATH 308, 309, 310, 312, 313, 341, 342</t>
   </si>
 </sst>
 </file>
@@ -11558,8 +11558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0A164B-708E-884A-B2CD-DB267B8D4A7F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11603,13 +11603,13 @@
         <v>349</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>379</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>376</v>
@@ -11626,13 +11626,13 @@
         <v>350</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>381</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>382</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>376</v>
@@ -11649,13 +11649,13 @@
         <v>351</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>384</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>385</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>376</v>
@@ -11672,13 +11672,13 @@
         <v>359</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>389</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>376</v>
@@ -11695,13 +11695,13 @@
         <v>352</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>390</v>
+        <v>448</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>376</v>
@@ -11714,9 +11714,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5605FB08-D761-1B4B-8F7E-F0D219ED9D4B}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -11778,18 +11780,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>307</v>
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="3">
-        <v>316</v>
+      <c r="B9">
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -11797,7 +11799,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="3">
-        <v>405</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -11805,7 +11807,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="3">
-        <v>340</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -11813,7 +11815,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <v>441</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -11821,7 +11823,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="3">
-        <v>360</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -11829,23 +11831,23 @@
         <v>2</v>
       </c>
       <c r="B14" s="3">
-        <v>461</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>302</v>
+        <v>2</v>
+      </c>
+      <c r="B15" s="3">
+        <v>461</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" s="3">
-        <v>303</v>
+      <c r="B16">
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -11853,7 +11855,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="3">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -11861,7 +11863,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="3">
-        <v>340</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -11869,7 +11871,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="3">
-        <v>441</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -11877,7 +11879,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="3">
-        <v>344</v>
+        <v>441</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -11885,23 +11887,23 @@
         <v>3</v>
       </c>
       <c r="B21" s="3">
-        <v>442</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>302</v>
+        <v>3</v>
+      </c>
+      <c r="B22" s="3">
+        <v>442</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
-      <c r="B23" s="3">
-        <v>303</v>
+      <c r="B23">
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -11909,7 +11911,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="3">
-        <v>344</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -11917,7 +11919,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="3">
-        <v>345</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -11925,7 +11927,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="3">
-        <v>360</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -11933,7 +11935,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="3">
-        <v>461</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -11941,7 +11943,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="3">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -11949,31 +11951,31 @@
         <v>4</v>
       </c>
       <c r="B29" s="3">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>5</v>
-      </c>
-      <c r="B30">
-        <v>310</v>
+        <v>4</v>
+      </c>
+      <c r="B30" s="3">
+        <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" s="3">
-        <v>341</v>
+        <v>462</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
-      <c r="B32" s="3">
-        <v>342</v>
+      <c r="B32">
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -11981,7 +11983,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="3">
-        <v>308</v>
+        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -11989,7 +11991,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="3">
-        <v>309</v>
+        <v>342</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -11997,7 +11999,7 @@
         <v>5</v>
       </c>
       <c r="B35" s="3">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -12005,6 +12007,22 @@
         <v>5</v>
       </c>
       <c r="B36" s="3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38" s="3">
         <v>313</v>
       </c>
     </row>
@@ -12076,25 +12094,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>402</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="119" x14ac:dyDescent="0.2">
@@ -12108,25 +12126,25 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>416</v>
-      </c>
       <c r="J3" s="7" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="221" x14ac:dyDescent="0.2">
@@ -12140,7 +12158,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>365</v>
@@ -12172,25 +12190,25 @@
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>420</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="119" x14ac:dyDescent="0.2">
@@ -12204,25 +12222,25 @@
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>433</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="119" x14ac:dyDescent="0.2">
@@ -12233,25 +12251,25 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>277</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="289" x14ac:dyDescent="0.2">
@@ -12265,25 +12283,25 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>408</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="187" x14ac:dyDescent="0.2">
@@ -12297,25 +12315,25 @@
         <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="204" x14ac:dyDescent="0.2">
@@ -12329,25 +12347,25 @@
         <v>5</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>438</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -19593,7 +19611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D05D007-E767-5440-814F-4CB4191763F7}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -19628,7 +19646,7 @@
         <v>348</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
@@ -19653,10 +19671,10 @@
         <v>299</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="200" customHeight="1" x14ac:dyDescent="0.2">
@@ -19667,10 +19685,10 @@
         <v>301</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>